<commit_message>
fixed some problems with fuel price projections. update so one large lookup or three separate.
</commit_message>
<xml_diff>
--- a/projections/aeo_projections_2022_2050.xlsx
+++ b/projections/aeo_projections_2022_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF5811FA-842B-46A1-A604-3BA845AF4BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08E8F73-101E-459D-8E50-7DB69D87EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="865" firstSheet="1" activeTab="1" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="865" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="fuel_price_factors_2022_2050" sheetId="9" r:id="rId1"/>
@@ -21,12 +21,25 @@
     <sheet name="aeo2019_key_indicators" sheetId="2" r:id="rId6"/>
     <sheet name="aeo2023_key_indicators" sheetId="1" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="421">
   <si>
     <t>Table 4.  Residential Sector Key Indicators and Consumption</t>
   </si>
@@ -1264,18 +1277,6 @@
     <t>AEO2023: Table 4 Residential Sector Key Indicators and Consumption</t>
   </si>
   <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -1293,14 +1294,23 @@
   <si>
     <t>projection_source</t>
   </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>AEO2023 Reference Case</t>
+  </si>
+  <si>
+    <t>AEO2022 Reference Case</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1797,7 +1807,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1806,26 +1816,23 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2203,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F5499C-249D-4660-AC39-83320A5A905A}">
   <dimension ref="A1:AG247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,113 +2221,113 @@
     <col min="3" max="3" width="31.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="D1" s="12">
+      <c r="D1" s="14">
         <v>2022</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="14">
         <v>2023</v>
       </c>
-      <c r="F1" s="12">
+      <c r="F1" s="14">
         <v>2024</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="14">
         <v>2025</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="14">
         <v>2026</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="14">
         <v>2027</v>
       </c>
-      <c r="J1" s="12">
+      <c r="J1" s="14">
         <v>2028</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="14">
         <v>2029</v>
       </c>
-      <c r="L1" s="12">
+      <c r="L1" s="14">
         <v>2030</v>
       </c>
-      <c r="M1" s="12">
+      <c r="M1" s="14">
         <v>2031</v>
       </c>
-      <c r="N1" s="12">
+      <c r="N1" s="14">
         <v>2032</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="14">
         <v>2033</v>
       </c>
-      <c r="P1" s="12">
+      <c r="P1" s="14">
         <v>2034</v>
       </c>
-      <c r="Q1" s="12">
+      <c r="Q1" s="14">
         <v>2035</v>
       </c>
-      <c r="R1" s="12">
+      <c r="R1" s="14">
         <v>2036</v>
       </c>
-      <c r="S1" s="12">
+      <c r="S1" s="14">
         <v>2037</v>
       </c>
-      <c r="T1" s="12">
+      <c r="T1" s="14">
         <v>2038</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="14">
         <v>2039</v>
       </c>
-      <c r="V1" s="12">
+      <c r="V1" s="14">
         <v>2040</v>
       </c>
-      <c r="W1" s="12">
+      <c r="W1" s="14">
         <v>2041</v>
       </c>
-      <c r="X1" s="12">
+      <c r="X1" s="14">
         <v>2042</v>
       </c>
-      <c r="Y1" s="12">
+      <c r="Y1" s="14">
         <v>2043</v>
       </c>
-      <c r="Z1" s="12">
+      <c r="Z1" s="14">
         <v>2044</v>
       </c>
-      <c r="AA1" s="12">
+      <c r="AA1" s="14">
         <v>2045</v>
       </c>
-      <c r="AB1" s="12">
+      <c r="AB1" s="14">
         <v>2046</v>
       </c>
-      <c r="AC1" s="12">
+      <c r="AC1" s="14">
         <v>2047</v>
       </c>
-      <c r="AD1" s="12">
+      <c r="AD1" s="14">
         <v>2048</v>
       </c>
-      <c r="AE1" s="12">
+      <c r="AE1" s="14">
         <v>2049</v>
       </c>
-      <c r="AF1" s="12">
+      <c r="AF1" s="14">
         <v>2050</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>401</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D2" s="5">
         <f>aeo_fuel_price_projections!$F2/aeo_fuel_price_projections!$F2</f>
@@ -2441,13 +2448,13 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>401</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D3" s="5">
         <f>aeo_fuel_price_projections!$F3/aeo_fuel_price_projections!$F3</f>
@@ -2568,7 +2575,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>401</v>
@@ -2695,7 +2702,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>401</v>
@@ -2822,7 +2829,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>401</v>
@@ -2949,7 +2956,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>401</v>
@@ -3076,13 +3083,13 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>402</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D8" s="5">
         <f>aeo_fuel_price_projections!$F8/aeo_fuel_price_projections!$F8</f>
@@ -3203,13 +3210,13 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>402</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D9" s="5">
         <f>aeo_fuel_price_projections!$F9/aeo_fuel_price_projections!$F9</f>
@@ -3330,7 +3337,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>402</v>
@@ -3457,7 +3464,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>402</v>
@@ -3584,7 +3591,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>402</v>
@@ -3711,7 +3718,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>402</v>
@@ -3838,13 +3845,13 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>403</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D14" s="5">
         <f>aeo_fuel_price_projections!$F14/aeo_fuel_price_projections!$F14</f>
@@ -3965,13 +3972,13 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>403</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D15" s="5">
         <f>aeo_fuel_price_projections!$F15/aeo_fuel_price_projections!$F15</f>
@@ -4092,7 +4099,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>403</v>
@@ -4219,7 +4226,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>403</v>
@@ -4346,7 +4353,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>403</v>
@@ -4473,7 +4480,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>403</v>
@@ -4600,13 +4607,13 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>404</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D20" s="5">
         <f>aeo_fuel_price_projections!$F20/aeo_fuel_price_projections!$F20</f>
@@ -4727,13 +4734,13 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>404</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D21" s="5">
         <f>aeo_fuel_price_projections!$F21/aeo_fuel_price_projections!$F21</f>
@@ -4854,7 +4861,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>404</v>
@@ -4981,7 +4988,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>404</v>
@@ -5108,7 +5115,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>404</v>
@@ -5235,7 +5242,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>404</v>
@@ -5368,7 +5375,7 @@
         <v>401</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D26" s="5">
         <f>aeo_fuel_price_projections!$F26/aeo_fuel_price_projections!$F26</f>
@@ -6003,7 +6010,7 @@
         <v>401</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D31" s="5">
         <f>aeo_fuel_price_projections!$F31/aeo_fuel_price_projections!$F31</f>
@@ -6131,7 +6138,7 @@
         <v>402</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D32" s="5">
         <f>aeo_fuel_price_projections!$F32/aeo_fuel_price_projections!$F32</f>
@@ -6771,7 +6778,7 @@
         <v>402</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D37" s="5">
         <f>aeo_fuel_price_projections!$F37/aeo_fuel_price_projections!$F37</f>
@@ -6899,7 +6906,7 @@
         <v>403</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D38" s="5">
         <f>aeo_fuel_price_projections!$F38/aeo_fuel_price_projections!$F38</f>
@@ -7539,7 +7546,7 @@
         <v>403</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D43" s="5">
         <f>aeo_fuel_price_projections!$F43/aeo_fuel_price_projections!$F43</f>
@@ -7667,7 +7674,7 @@
         <v>404</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D44" s="5">
         <f>aeo_fuel_price_projections!$F44/aeo_fuel_price_projections!$F44</f>
@@ -8307,7 +8314,7 @@
         <v>404</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D49" s="5">
         <f>aeo_fuel_price_projections!$F49/aeo_fuel_price_projections!$F49</f>
@@ -8435,7 +8442,7 @@
         <v>401</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D50" s="5">
         <f>aeo_fuel_price_projections!$F50/aeo_fuel_price_projections!$F50</f>
@@ -9073,7 +9080,7 @@
         <v>401</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D55" s="5">
         <f>aeo_fuel_price_projections!$F55/aeo_fuel_price_projections!$F55</f>
@@ -9200,7 +9207,7 @@
         <v>402</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D56" s="5">
         <f>aeo_fuel_price_projections!$F56/aeo_fuel_price_projections!$F56</f>
@@ -9835,7 +9842,7 @@
         <v>402</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D61" s="5">
         <f>aeo_fuel_price_projections!$F61/aeo_fuel_price_projections!$F61</f>
@@ -9962,7 +9969,7 @@
         <v>403</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D62" s="5">
         <f>aeo_fuel_price_projections!$F62/aeo_fuel_price_projections!$F62</f>
@@ -10597,7 +10604,7 @@
         <v>403</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D67" s="5">
         <f>aeo_fuel_price_projections!$F67/aeo_fuel_price_projections!$F67</f>
@@ -10724,7 +10731,7 @@
         <v>404</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D68" s="5">
         <f>aeo_fuel_price_projections!$F68/aeo_fuel_price_projections!$F68</f>
@@ -11359,7 +11366,7 @@
         <v>404</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D73" s="5">
         <f>aeo_fuel_price_projections!$F73/aeo_fuel_price_projections!$F73</f>
@@ -11486,7 +11493,7 @@
         <v>401</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D74" s="5">
         <f>aeo_fuel_price_projections!$F74/aeo_fuel_price_projections!$F74</f>
@@ -12121,7 +12128,7 @@
         <v>401</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D79" s="5">
         <f>aeo_fuel_price_projections!$F79/aeo_fuel_price_projections!$F79</f>
@@ -12248,7 +12255,7 @@
         <v>402</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D80" s="5">
         <f>aeo_fuel_price_projections!$F80/aeo_fuel_price_projections!$F80</f>
@@ -12883,7 +12890,7 @@
         <v>402</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D85" s="5">
         <f>aeo_fuel_price_projections!$F85/aeo_fuel_price_projections!$F85</f>
@@ -13010,7 +13017,7 @@
         <v>403</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D86" s="5">
         <f>aeo_fuel_price_projections!$F86/aeo_fuel_price_projections!$F86</f>
@@ -13645,7 +13652,7 @@
         <v>403</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D91" s="5">
         <f>aeo_fuel_price_projections!$F91/aeo_fuel_price_projections!$F91</f>
@@ -13772,7 +13779,7 @@
         <v>404</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D92" s="5">
         <f>aeo_fuel_price_projections!$F92/aeo_fuel_price_projections!$F92</f>
@@ -14407,7 +14414,7 @@
         <v>404</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D97" s="5">
         <f>aeo_fuel_price_projections!$F97/aeo_fuel_price_projections!$F97</f>
@@ -14534,7 +14541,7 @@
         <v>401</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D98" s="5">
         <f>aeo_fuel_price_projections!$F98/aeo_fuel_price_projections!$F98</f>
@@ -15169,7 +15176,7 @@
         <v>401</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D103" s="5">
         <f>aeo_fuel_price_projections!$F103/aeo_fuel_price_projections!$F103</f>
@@ -15296,7 +15303,7 @@
         <v>402</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D104" s="5">
         <f>aeo_fuel_price_projections!$F104/aeo_fuel_price_projections!$F104</f>
@@ -15931,7 +15938,7 @@
         <v>402</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D109" s="5">
         <f>aeo_fuel_price_projections!$F109/aeo_fuel_price_projections!$F109</f>
@@ -16058,7 +16065,7 @@
         <v>403</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D110" s="5">
         <f>aeo_fuel_price_projections!$F110/aeo_fuel_price_projections!$F110</f>
@@ -16693,7 +16700,7 @@
         <v>403</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D115" s="5">
         <f>aeo_fuel_price_projections!$F115/aeo_fuel_price_projections!$F115</f>
@@ -16820,7 +16827,7 @@
         <v>404</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D116" s="5">
         <f>aeo_fuel_price_projections!$F116/aeo_fuel_price_projections!$F116</f>
@@ -17455,7 +17462,7 @@
         <v>404</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D121" s="5">
         <f>aeo_fuel_price_projections!$F121/aeo_fuel_price_projections!$F121</f>
@@ -17582,7 +17589,7 @@
         <v>401</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D122" s="5">
         <f>aeo_fuel_price_projections!$F122/aeo_fuel_price_projections!$F122</f>
@@ -18217,7 +18224,7 @@
         <v>401</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D127" s="5">
         <f>aeo_fuel_price_projections!$F127/aeo_fuel_price_projections!$F127</f>
@@ -18344,7 +18351,7 @@
         <v>402</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D128" s="5">
         <f>aeo_fuel_price_projections!$F128/aeo_fuel_price_projections!$F128</f>
@@ -18979,7 +18986,7 @@
         <v>402</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D133" s="5">
         <f>aeo_fuel_price_projections!$F133/aeo_fuel_price_projections!$F133</f>
@@ -19106,7 +19113,7 @@
         <v>403</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D134" s="5">
         <f>aeo_fuel_price_projections!$F134/aeo_fuel_price_projections!$F134</f>
@@ -19741,7 +19748,7 @@
         <v>403</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D139" s="5">
         <f>aeo_fuel_price_projections!$F139/aeo_fuel_price_projections!$F139</f>
@@ -19868,7 +19875,7 @@
         <v>404</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D140" s="5">
         <f>aeo_fuel_price_projections!$F140/aeo_fuel_price_projections!$F140</f>
@@ -20503,7 +20510,7 @@
         <v>404</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D145" s="5">
         <f>aeo_fuel_price_projections!$F145/aeo_fuel_price_projections!$F145</f>
@@ -20630,7 +20637,7 @@
         <v>401</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D146" s="5">
         <f>aeo_fuel_price_projections!$F146/aeo_fuel_price_projections!$F146</f>
@@ -21265,7 +21272,7 @@
         <v>401</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D151" s="5">
         <f>aeo_fuel_price_projections!$F151/aeo_fuel_price_projections!$F151</f>
@@ -21392,7 +21399,7 @@
         <v>402</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D152" s="5">
         <f>aeo_fuel_price_projections!$F152/aeo_fuel_price_projections!$F152</f>
@@ -22027,7 +22034,7 @@
         <v>402</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D157" s="5">
         <f>aeo_fuel_price_projections!$F157/aeo_fuel_price_projections!$F157</f>
@@ -22154,7 +22161,7 @@
         <v>403</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D158" s="5">
         <f>aeo_fuel_price_projections!$F158/aeo_fuel_price_projections!$F158</f>
@@ -22789,7 +22796,7 @@
         <v>403</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D163" s="5">
         <f>aeo_fuel_price_projections!$F163/aeo_fuel_price_projections!$F163</f>
@@ -22916,7 +22923,7 @@
         <v>404</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D164" s="5">
         <f>aeo_fuel_price_projections!$F164/aeo_fuel_price_projections!$F164</f>
@@ -23551,7 +23558,7 @@
         <v>404</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D169" s="5">
         <f>aeo_fuel_price_projections!$F169/aeo_fuel_price_projections!$F169</f>
@@ -23678,7 +23685,7 @@
         <v>401</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D170" s="5">
         <f>aeo_fuel_price_projections!$F170/aeo_fuel_price_projections!$F170</f>
@@ -24313,7 +24320,7 @@
         <v>401</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D175" s="5">
         <f>aeo_fuel_price_projections!$F175/aeo_fuel_price_projections!$F175</f>
@@ -24440,7 +24447,7 @@
         <v>402</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D176" s="5">
         <f>aeo_fuel_price_projections!$F176/aeo_fuel_price_projections!$F176</f>
@@ -25075,7 +25082,7 @@
         <v>402</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D181" s="5">
         <f>aeo_fuel_price_projections!$F181/aeo_fuel_price_projections!$F181</f>
@@ -25202,7 +25209,7 @@
         <v>403</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D182" s="5">
         <f>aeo_fuel_price_projections!$F182/aeo_fuel_price_projections!$F182</f>
@@ -25837,7 +25844,7 @@
         <v>403</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D187" s="5">
         <f>aeo_fuel_price_projections!$F187/aeo_fuel_price_projections!$F187</f>
@@ -25964,7 +25971,7 @@
         <v>404</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D188" s="5">
         <f>aeo_fuel_price_projections!$F188/aeo_fuel_price_projections!$F188</f>
@@ -26599,7 +26606,7 @@
         <v>404</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D193" s="5">
         <f>aeo_fuel_price_projections!$F193/aeo_fuel_price_projections!$F193</f>
@@ -26726,7 +26733,7 @@
         <v>401</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D194" s="5">
         <f>aeo_fuel_price_projections!$F194/aeo_fuel_price_projections!$F194</f>
@@ -27361,7 +27368,7 @@
         <v>401</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D199" s="5">
         <f>aeo_fuel_price_projections!$F199/aeo_fuel_price_projections!$F199</f>
@@ -27488,7 +27495,7 @@
         <v>402</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D200" s="5">
         <f>aeo_fuel_price_projections!$F200/aeo_fuel_price_projections!$F200</f>
@@ -28123,7 +28130,7 @@
         <v>402</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D205" s="5">
         <f>aeo_fuel_price_projections!$F205/aeo_fuel_price_projections!$F205</f>
@@ -28250,7 +28257,7 @@
         <v>403</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D206" s="5">
         <f>aeo_fuel_price_projections!$F206/aeo_fuel_price_projections!$F206</f>
@@ -28885,7 +28892,7 @@
         <v>403</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D211" s="5">
         <f>aeo_fuel_price_projections!$F211/aeo_fuel_price_projections!$F211</f>
@@ -29012,7 +29019,7 @@
         <v>404</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D212" s="5">
         <f>aeo_fuel_price_projections!$F212/aeo_fuel_price_projections!$F212</f>
@@ -29647,7 +29654,7 @@
         <v>404</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D217" s="5">
         <f>aeo_fuel_price_projections!$F217/aeo_fuel_price_projections!$F217</f>
@@ -29774,7 +29781,7 @@
         <v>401</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D218" s="5">
         <f>aeo_fuel_price_projections!$F218/aeo_fuel_price_projections!$F218</f>
@@ -30409,7 +30416,7 @@
         <v>401</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D223" s="5">
         <f>aeo_fuel_price_projections!$F223/aeo_fuel_price_projections!$F223</f>
@@ -30536,7 +30543,7 @@
         <v>402</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D224" s="5">
         <f>aeo_fuel_price_projections!$F224/aeo_fuel_price_projections!$F224</f>
@@ -31171,7 +31178,7 @@
         <v>402</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D229" s="5">
         <f>aeo_fuel_price_projections!$F229/aeo_fuel_price_projections!$F229</f>
@@ -31298,7 +31305,7 @@
         <v>403</v>
       </c>
       <c r="C230" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D230" s="5">
         <f>aeo_fuel_price_projections!$F230/aeo_fuel_price_projections!$F230</f>
@@ -31933,7 +31940,7 @@
         <v>403</v>
       </c>
       <c r="C235" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D235" s="5">
         <f>aeo_fuel_price_projections!$F235/aeo_fuel_price_projections!$F235</f>
@@ -32060,7 +32067,7 @@
         <v>404</v>
       </c>
       <c r="C236" s="10" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="D236" s="5">
         <f>aeo_fuel_price_projections!$F236/aeo_fuel_price_projections!$F236</f>
@@ -32695,7 +32702,7 @@
         <v>404</v>
       </c>
       <c r="C241" s="10" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D241" s="5">
         <f>aeo_fuel_price_projections!$F241/aeo_fuel_price_projections!$F241</f>
@@ -33003,8 +33010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F19DDE-A522-4386-88E1-4C69D68CACB1}">
   <dimension ref="A1:AI241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33015,107 +33022,107 @@
     <col min="5" max="5" width="13.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="12">
+      <c r="F1" s="14">
         <v>2022</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="14">
         <v>2023</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="14">
         <v>2024</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="14">
         <v>2025</v>
       </c>
-      <c r="J1" s="12">
+      <c r="J1" s="14">
         <v>2026</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="14">
         <v>2027</v>
       </c>
-      <c r="L1" s="12">
+      <c r="L1" s="14">
         <v>2028</v>
       </c>
-      <c r="M1" s="12">
+      <c r="M1" s="14">
         <v>2029</v>
       </c>
-      <c r="N1" s="12">
+      <c r="N1" s="14">
         <v>2030</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="14">
         <v>2031</v>
       </c>
-      <c r="P1" s="12">
+      <c r="P1" s="14">
         <v>2032</v>
       </c>
-      <c r="Q1" s="12">
+      <c r="Q1" s="14">
         <v>2033</v>
       </c>
-      <c r="R1" s="12">
+      <c r="R1" s="14">
         <v>2034</v>
       </c>
-      <c r="S1" s="12">
+      <c r="S1" s="14">
         <v>2035</v>
       </c>
-      <c r="T1" s="12">
+      <c r="T1" s="14">
         <v>2036</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="14">
         <v>2037</v>
       </c>
-      <c r="V1" s="12">
+      <c r="V1" s="14">
         <v>2038</v>
       </c>
-      <c r="W1" s="12">
+      <c r="W1" s="14">
         <v>2039</v>
       </c>
-      <c r="X1" s="12">
+      <c r="X1" s="14">
         <v>2040</v>
       </c>
-      <c r="Y1" s="12">
+      <c r="Y1" s="14">
         <v>2041</v>
       </c>
-      <c r="Z1" s="12">
+      <c r="Z1" s="14">
         <v>2042</v>
       </c>
-      <c r="AA1" s="12">
+      <c r="AA1" s="14">
         <v>2043</v>
       </c>
-      <c r="AB1" s="12">
+      <c r="AB1" s="14">
         <v>2044</v>
       </c>
-      <c r="AC1" s="12">
+      <c r="AC1" s="14">
         <v>2045</v>
       </c>
-      <c r="AD1" s="12">
+      <c r="AD1" s="14">
         <v>2046</v>
       </c>
-      <c r="AE1" s="12">
+      <c r="AE1" s="14">
         <v>2047</v>
       </c>
-      <c r="AF1" s="12">
+      <c r="AF1" s="14">
         <v>2048</v>
       </c>
-      <c r="AG1" s="12">
+      <c r="AG1" s="14">
         <v>2049</v>
       </c>
-      <c r="AH1" s="12">
+      <c r="AH1" s="14">
         <v>2050</v>
       </c>
     </row>
@@ -58112,7 +58119,7 @@
   <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58123,243 +58130,243 @@
     <col min="5" max="5" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>415</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="F1" s="12">
+      <c r="B1" s="14">
+        <v>2018</v>
+      </c>
+      <c r="C1" s="14">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="14">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="14">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="14">
         <v>2022</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="14">
         <v>2023</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="14">
         <v>2024</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="14">
         <v>2025</v>
       </c>
-      <c r="J1" s="12">
+      <c r="J1" s="14">
         <v>2026</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="14">
         <v>2027</v>
       </c>
-      <c r="L1" s="12">
+      <c r="L1" s="14">
         <v>2028</v>
       </c>
-      <c r="M1" s="12">
+      <c r="M1" s="14">
         <v>2029</v>
       </c>
-      <c r="N1" s="12">
+      <c r="N1" s="14">
         <v>2030</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="14">
         <v>2031</v>
       </c>
-      <c r="P1" s="12">
+      <c r="P1" s="14">
         <v>2032</v>
       </c>
-      <c r="Q1" s="12">
+      <c r="Q1" s="14">
         <v>2033</v>
       </c>
-      <c r="R1" s="12">
+      <c r="R1" s="14">
         <v>2034</v>
       </c>
-      <c r="S1" s="12">
+      <c r="S1" s="14">
         <v>2035</v>
       </c>
-      <c r="T1" s="12">
+      <c r="T1" s="14">
         <v>2036</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="14">
         <v>2037</v>
       </c>
-      <c r="V1" s="12">
+      <c r="V1" s="14">
         <v>2038</v>
       </c>
-      <c r="W1" s="12">
+      <c r="W1" s="14">
         <v>2039</v>
       </c>
-      <c r="X1" s="12">
+      <c r="X1" s="14">
         <v>2040</v>
       </c>
-      <c r="Y1" s="12">
+      <c r="Y1" s="14">
         <v>2041</v>
       </c>
-      <c r="Z1" s="12">
+      <c r="Z1" s="14">
         <v>2042</v>
       </c>
-      <c r="AA1" s="12">
+      <c r="AA1" s="14">
         <v>2043</v>
       </c>
-      <c r="AB1" s="12">
+      <c r="AB1" s="14">
         <v>2044</v>
       </c>
-      <c r="AC1" s="12">
+      <c r="AC1" s="14">
         <v>2045</v>
       </c>
-      <c r="AD1" s="12">
+      <c r="AD1" s="14">
         <v>2046</v>
       </c>
-      <c r="AE1" s="12">
+      <c r="AE1" s="14">
         <v>2047</v>
       </c>
-      <c r="AF1" s="12">
+      <c r="AF1" s="14">
         <v>2048</v>
       </c>
-      <c r="AG1" s="12">
+      <c r="AG1" s="14">
         <v>2049</v>
       </c>
-      <c r="AH1" s="12">
+      <c r="AH1" s="14">
         <v>2050</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="B2" s="15">
+        <v>414</v>
+      </c>
+      <c r="B2" s="13">
         <f>aeo_hdd_projections!$F2/aeo_hdd_projections!$F2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="13">
         <f>aeo_hdd_projections!G2/aeo_hdd_projections!$F2</f>
         <v>1.0060591936611512</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="13">
         <f>aeo_hdd_projections!H2/aeo_hdd_projections!$F2</f>
         <v>0.91214169191330696</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <f>aeo_hdd_projections!I2/aeo_hdd_projections!$F2</f>
         <v>0.91680261011419251</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="13">
         <f>aeo_hdd_projections!J2/aeo_hdd_projections!$F2</f>
         <v>0.98685941971568403</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="13">
         <f>aeo_hdd_projections!K2/aeo_hdd_projections!$F2</f>
         <v>0.98965710836634824</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="13">
         <f>aeo_hdd_projections!L2/aeo_hdd_projections!$F2</f>
         <v>0.92661523118154276</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <f>aeo_hdd_projections!M2/aeo_hdd_projections!$F2</f>
         <v>0.92220476905150317</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="13">
         <f>aeo_hdd_projections!N2/aeo_hdd_projections!$F2</f>
         <v>0.91786098904684221</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="13">
         <f>aeo_hdd_projections!O2/aeo_hdd_projections!$F2</f>
         <v>0.91354269843859237</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="13">
         <f>aeo_hdd_projections!P2/aeo_hdd_projections!$F2</f>
         <v>0.90917177907247726</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="13">
         <f>aeo_hdd_projections!Q2/aeo_hdd_projections!$F2</f>
         <v>0.90480586646469352</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="13">
         <f>aeo_hdd_projections!R2/aeo_hdd_projections!$F2</f>
         <v>0.90044518830109532</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="13">
         <f>aeo_hdd_projections!S2/aeo_hdd_projections!$F2</f>
         <v>0.89610556164064314</v>
       </c>
-      <c r="P2" s="15">
+      <c r="P2" s="13">
         <f>aeo_hdd_projections!T2/aeo_hdd_projections!$F2</f>
         <v>0.89177959007224428</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="13">
         <f>aeo_hdd_projections!U2/aeo_hdd_projections!$F2</f>
         <v>0.8874326238639012</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="13">
         <f>aeo_hdd_projections!V2/aeo_hdd_projections!$F2</f>
         <v>0.88311632439990673</v>
       </c>
-      <c r="S2" s="15">
+      <c r="S2" s="13">
         <f>aeo_hdd_projections!W2/aeo_hdd_projections!$F2</f>
         <v>0.87877447890934512</v>
       </c>
-      <c r="T2" s="15">
+      <c r="T2" s="13">
         <f>aeo_hdd_projections!X2/aeo_hdd_projections!$F2</f>
         <v>0.87439593544628291</v>
       </c>
-      <c r="U2" s="15">
+      <c r="U2" s="13">
         <f>aeo_hdd_projections!Y2/aeo_hdd_projections!$F2</f>
         <v>0.8701421647634584</v>
       </c>
-      <c r="V2" s="15">
+      <c r="V2" s="13">
         <f>aeo_hdd_projections!Z2/aeo_hdd_projections!$F2</f>
         <v>0.86583678955954324</v>
       </c>
-      <c r="W2" s="15">
+      <c r="W2" s="13">
         <f>aeo_hdd_projections!AA2/aeo_hdd_projections!$F2</f>
         <v>0.86146057888604055</v>
       </c>
-      <c r="X2" s="15">
+      <c r="X2" s="13">
         <f>aeo_hdd_projections!AB2/aeo_hdd_projections!$F2</f>
         <v>0.85717022419016542</v>
       </c>
-      <c r="Y2" s="15">
+      <c r="Y2" s="13">
         <f>aeo_hdd_projections!AC2/aeo_hdd_projections!$F2</f>
         <v>0.85291321044045676</v>
       </c>
-      <c r="Z2" s="15">
+      <c r="Z2" s="13">
         <f>aeo_hdd_projections!AD2/aeo_hdd_projections!$F2</f>
         <v>0.84861232999300862</v>
       </c>
-      <c r="AA2" s="15">
+      <c r="AA2" s="13">
         <f>aeo_hdd_projections!AE2/aeo_hdd_projections!$F2</f>
         <v>0.8443018340713121</v>
       </c>
-      <c r="AB2" s="15">
+      <c r="AB2" s="13">
         <f>aeo_hdd_projections!AF2/aeo_hdd_projections!$F2</f>
         <v>0.8399903710090888</v>
       </c>
-      <c r="AC2" s="15">
+      <c r="AC2" s="13">
         <f>aeo_hdd_projections!AG2/aeo_hdd_projections!$F2</f>
         <v>0.83569552132370073</v>
       </c>
-      <c r="AD2" s="15">
+      <c r="AD2" s="13">
         <f>aeo_hdd_projections!AH2/aeo_hdd_projections!$F2</f>
         <v>0.83143799557212772</v>
       </c>
-      <c r="AE2" s="15">
+      <c r="AE2" s="13">
         <f>aeo_hdd_projections!AI2/aeo_hdd_projections!$F2</f>
         <v>0.82720999883477042</v>
       </c>
-      <c r="AF2" s="15">
+      <c r="AF2" s="13">
         <f>aeo_hdd_projections!AJ2/aeo_hdd_projections!$F2</f>
         <v>0.82298046609182007</v>
       </c>
-      <c r="AG2" s="15">
+      <c r="AG2" s="13">
         <f>aeo_hdd_projections!AK2/aeo_hdd_projections!$F2</f>
         <v>0.8188027084595666</v>
       </c>
-      <c r="AH2" s="15">
+      <c r="AH2" s="13">
         <f>aeo_hdd_projections!AL2/aeo_hdd_projections!$F2</f>
         <v>0.81465271615008161</v>
       </c>
@@ -58368,135 +58375,135 @@
       <c r="A3" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <f>aeo_hdd_projections!$F3/aeo_hdd_projections!$F3</f>
         <v>1</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <f>aeo_hdd_projections!G3/aeo_hdd_projections!$F3</f>
         <v>0.99891202984146721</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <f>aeo_hdd_projections!H3/aeo_hdd_projections!$F3</f>
         <v>0.91000932545850166</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="13">
         <f>aeo_hdd_projections!I3/aeo_hdd_projections!$F3</f>
         <v>0.89322350015542429</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <f>aeo_hdd_projections!J3/aeo_hdd_projections!$F3</f>
         <v>0.99891202984146721</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <f>aeo_hdd_projections!K3/aeo_hdd_projections!$F3</f>
         <v>0.98010568852968605</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <f>aeo_hdd_projections!L3/aeo_hdd_projections!$F3</f>
         <v>0.92974821262045382</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <f>aeo_hdd_projections!M3/aeo_hdd_projections!$F3</f>
         <v>0.92741684799502644</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="13">
         <f>aeo_hdd_projections!N3/aeo_hdd_projections!$F3</f>
         <v>0.92524090767796086</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="13">
         <f>aeo_hdd_projections!O3/aeo_hdd_projections!$F3</f>
         <v>0.92290954305253337</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="13">
         <f>aeo_hdd_projections!P3/aeo_hdd_projections!$F3</f>
         <v>0.92057817842710599</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="13">
         <f>aeo_hdd_projections!Q3/aeo_hdd_projections!$F3</f>
         <v>0.91824681380167861</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="13">
         <f>aeo_hdd_projections!R3/aeo_hdd_projections!$F3</f>
         <v>0.91591544917625112</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="13">
         <f>aeo_hdd_projections!S3/aeo_hdd_projections!$F3</f>
         <v>0.91373950885918553</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="13">
         <f>aeo_hdd_projections!T3/aeo_hdd_projections!$F3</f>
         <v>0.91140814423375816</v>
       </c>
-      <c r="Q3" s="15">
+      <c r="Q3" s="13">
         <f>aeo_hdd_projections!U3/aeo_hdd_projections!$F3</f>
         <v>0.90907677960833078</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="13">
         <f>aeo_hdd_projections!V3/aeo_hdd_projections!$F3</f>
         <v>0.90674541498290329</v>
       </c>
-      <c r="S3" s="15">
+      <c r="S3" s="13">
         <f>aeo_hdd_projections!W3/aeo_hdd_projections!$F3</f>
         <v>0.90441405035747591</v>
       </c>
-      <c r="T3" s="15">
+      <c r="T3" s="13">
         <f>aeo_hdd_projections!X3/aeo_hdd_projections!$F3</f>
         <v>0.90208268573204853</v>
       </c>
-      <c r="U3" s="15">
+      <c r="U3" s="13">
         <f>aeo_hdd_projections!Y3/aeo_hdd_projections!$F3</f>
         <v>0.89990674541498294</v>
       </c>
-      <c r="V3" s="15">
+      <c r="V3" s="13">
         <f>aeo_hdd_projections!Z3/aeo_hdd_projections!$F3</f>
         <v>0.89757538078955545</v>
       </c>
-      <c r="W3" s="15">
+      <c r="W3" s="13">
         <f>aeo_hdd_projections!AA3/aeo_hdd_projections!$F3</f>
         <v>0.89524401616412808</v>
       </c>
-      <c r="X3" s="15">
+      <c r="X3" s="13">
         <f>aeo_hdd_projections!AB3/aeo_hdd_projections!$F3</f>
         <v>0.8929126515387007</v>
       </c>
-      <c r="Y3" s="15">
+      <c r="Y3" s="13">
         <f>aeo_hdd_projections!AC3/aeo_hdd_projections!$F3</f>
         <v>0.89058128691327321</v>
       </c>
-      <c r="Z3" s="15">
+      <c r="Z3" s="13">
         <f>aeo_hdd_projections!AD3/aeo_hdd_projections!$F3</f>
         <v>0.88824992228784583</v>
       </c>
-      <c r="AA3" s="15">
+      <c r="AA3" s="13">
         <f>aeo_hdd_projections!AE3/aeo_hdd_projections!$F3</f>
         <v>0.88607398197078024</v>
       </c>
-      <c r="AB3" s="15">
+      <c r="AB3" s="13">
         <f>aeo_hdd_projections!AF3/aeo_hdd_projections!$F3</f>
         <v>0.88374261734535287</v>
       </c>
-      <c r="AC3" s="15">
+      <c r="AC3" s="13">
         <f>aeo_hdd_projections!AG3/aeo_hdd_projections!$F3</f>
         <v>0.88141125271992538</v>
       </c>
-      <c r="AD3" s="15">
+      <c r="AD3" s="13">
         <f>aeo_hdd_projections!AH3/aeo_hdd_projections!$F3</f>
         <v>0.879079888094498</v>
       </c>
-      <c r="AE3" s="15">
+      <c r="AE3" s="13">
         <f>aeo_hdd_projections!AI3/aeo_hdd_projections!$F3</f>
         <v>0.87674852346907062</v>
       </c>
-      <c r="AF3" s="15">
+      <c r="AF3" s="13">
         <f>aeo_hdd_projections!AJ3/aeo_hdd_projections!$F3</f>
         <v>0.87441715884364313</v>
       </c>
-      <c r="AG3" s="15">
+      <c r="AG3" s="13">
         <f>aeo_hdd_projections!AK3/aeo_hdd_projections!$F3</f>
         <v>0.87208579421821575</v>
       </c>
-      <c r="AH3" s="15">
+      <c r="AH3" s="13">
         <f>aeo_hdd_projections!AL3/aeo_hdd_projections!$F3</f>
         <v>0.86990985390115017</v>
       </c>
@@ -58505,135 +58512,135 @@
       <c r="A4" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <f>aeo_hdd_projections!$F4/aeo_hdd_projections!$F4</f>
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <f>aeo_hdd_projections!G4/aeo_hdd_projections!$F4</f>
         <v>0.91434320206956021</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <f>aeo_hdd_projections!H4/aeo_hdd_projections!$F4</f>
         <v>0.88071284851968956</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <f>aeo_hdd_projections!I4/aeo_hdd_projections!$F4</f>
         <v>0.91003161828111523</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <f>aeo_hdd_projections!J4/aeo_hdd_projections!$F4</f>
         <v>1.0022995113538373</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <f>aeo_hdd_projections!K4/aeo_hdd_projections!$F4</f>
         <v>0.98936475998850248</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <f>aeo_hdd_projections!L4/aeo_hdd_projections!$F4</f>
         <v>0.91405576315033055</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <f>aeo_hdd_projections!M4/aeo_hdd_projections!$F4</f>
         <v>0.91060649611957456</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="13">
         <f>aeo_hdd_projections!N4/aeo_hdd_projections!$F4</f>
         <v>0.90715722908881857</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="13">
         <f>aeo_hdd_projections!O4/aeo_hdd_projections!$F4</f>
         <v>0.9037079620580627</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="13">
         <f>aeo_hdd_projections!P4/aeo_hdd_projections!$F4</f>
         <v>0.89997125610807704</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="13">
         <f>aeo_hdd_projections!Q4/aeo_hdd_projections!$F4</f>
         <v>0.89652198907732106</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="13">
         <f>aeo_hdd_projections!R4/aeo_hdd_projections!$F4</f>
         <v>0.89278528312733541</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="13">
         <f>aeo_hdd_projections!S4/aeo_hdd_projections!$F4</f>
         <v>0.88933601609657953</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="13">
         <f>aeo_hdd_projections!T4/aeo_hdd_projections!$F4</f>
         <v>0.88559931014659388</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="13">
         <f>aeo_hdd_projections!U4/aeo_hdd_projections!$F4</f>
         <v>0.88215004311583789</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="13">
         <f>aeo_hdd_projections!V4/aeo_hdd_projections!$F4</f>
         <v>0.87841333716585224</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="13">
         <f>aeo_hdd_projections!W4/aeo_hdd_projections!$F4</f>
         <v>0.87467663121586658</v>
       </c>
-      <c r="T4" s="15">
+      <c r="T4" s="13">
         <f>aeo_hdd_projections!X4/aeo_hdd_projections!$F4</f>
         <v>0.87122736418511071</v>
       </c>
-      <c r="U4" s="15">
+      <c r="U4" s="13">
         <f>aeo_hdd_projections!Y4/aeo_hdd_projections!$F4</f>
         <v>0.86749065823512506</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="13">
         <f>aeo_hdd_projections!Z4/aeo_hdd_projections!$F4</f>
         <v>0.8637539522851394</v>
       </c>
-      <c r="W4" s="15">
+      <c r="W4" s="13">
         <f>aeo_hdd_projections!AA4/aeo_hdd_projections!$F4</f>
         <v>0.86001724633515375</v>
       </c>
-      <c r="X4" s="15">
+      <c r="X4" s="13">
         <f>aeo_hdd_projections!AB4/aeo_hdd_projections!$F4</f>
         <v>0.85656797930439776</v>
       </c>
-      <c r="Y4" s="15">
+      <c r="Y4" s="13">
         <f>aeo_hdd_projections!AC4/aeo_hdd_projections!$F4</f>
         <v>0.85283127335441222</v>
       </c>
-      <c r="Z4" s="15">
+      <c r="Z4" s="13">
         <f>aeo_hdd_projections!AD4/aeo_hdd_projections!$F4</f>
         <v>0.84909456740442657</v>
       </c>
-      <c r="AA4" s="15">
+      <c r="AA4" s="13">
         <f>aeo_hdd_projections!AE4/aeo_hdd_projections!$F4</f>
         <v>0.84535786145444092</v>
       </c>
-      <c r="AB4" s="15">
+      <c r="AB4" s="13">
         <f>aeo_hdd_projections!AF4/aeo_hdd_projections!$F4</f>
         <v>0.84190859442368493</v>
       </c>
-      <c r="AC4" s="15">
+      <c r="AC4" s="13">
         <f>aeo_hdd_projections!AG4/aeo_hdd_projections!$F4</f>
         <v>0.83817188847369939</v>
       </c>
-      <c r="AD4" s="15">
+      <c r="AD4" s="13">
         <f>aeo_hdd_projections!AH4/aeo_hdd_projections!$F4</f>
         <v>0.83443518252371374</v>
       </c>
-      <c r="AE4" s="15">
+      <c r="AE4" s="13">
         <f>aeo_hdd_projections!AI4/aeo_hdd_projections!$F4</f>
         <v>0.83069847657372808</v>
       </c>
-      <c r="AF4" s="15">
+      <c r="AF4" s="13">
         <f>aeo_hdd_projections!AJ4/aeo_hdd_projections!$F4</f>
         <v>0.82696177062374243</v>
       </c>
-      <c r="AG4" s="15">
+      <c r="AG4" s="13">
         <f>aeo_hdd_projections!AK4/aeo_hdd_projections!$F4</f>
         <v>0.82351250359298644</v>
       </c>
-      <c r="AH4" s="15">
+      <c r="AH4" s="13">
         <f>aeo_hdd_projections!AL4/aeo_hdd_projections!$F4</f>
         <v>0.8197757976430009</v>
       </c>
@@ -58642,135 +58649,135 @@
       <c r="A5" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="13">
         <f>aeo_hdd_projections!$F5/aeo_hdd_projections!$F5</f>
         <v>1</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <f>aeo_hdd_projections!G5/aeo_hdd_projections!$F5</f>
         <v>0.99427977119084765</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <f>aeo_hdd_projections!H5/aeo_hdd_projections!$F5</f>
         <v>0.90119604784191365</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <f>aeo_hdd_projections!I5/aeo_hdd_projections!$F5</f>
         <v>0.91211648465938633</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="13">
         <f>aeo_hdd_projections!J5/aeo_hdd_projections!$F5</f>
         <v>0.99531981279251169</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <f>aeo_hdd_projections!K5/aeo_hdd_projections!$F5</f>
         <v>1.0017334026694402</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="13">
         <f>aeo_hdd_projections!L5/aeo_hdd_projections!$F5</f>
         <v>0.92702374761657136</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <f>aeo_hdd_projections!M5/aeo_hdd_projections!$F5</f>
         <v>0.92303692147685912</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="13">
         <f>aeo_hdd_projections!N5/aeo_hdd_projections!$F5</f>
         <v>0.91922343560409081</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="13">
         <f>aeo_hdd_projections!O5/aeo_hdd_projections!$F5</f>
         <v>0.91540994973132261</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="13">
         <f>aeo_hdd_projections!P5/aeo_hdd_projections!$F5</f>
         <v>0.91159646385855431</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="13">
         <f>aeo_hdd_projections!Q5/aeo_hdd_projections!$F5</f>
         <v>0.90760963771884207</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="13">
         <f>aeo_hdd_projections!R5/aeo_hdd_projections!$F5</f>
         <v>0.90379615184607387</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="13">
         <f>aeo_hdd_projections!S5/aeo_hdd_projections!$F5</f>
         <v>0.89998266597330556</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="13">
         <f>aeo_hdd_projections!T5/aeo_hdd_projections!$F5</f>
         <v>0.89599583983359332</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="13">
         <f>aeo_hdd_projections!U5/aeo_hdd_projections!$F5</f>
         <v>0.89218235396082513</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="13">
         <f>aeo_hdd_projections!V5/aeo_hdd_projections!$F5</f>
         <v>0.88836886808805682</v>
       </c>
-      <c r="S5" s="15">
+      <c r="S5" s="13">
         <f>aeo_hdd_projections!W5/aeo_hdd_projections!$F5</f>
         <v>0.88438204194834458</v>
       </c>
-      <c r="T5" s="15">
+      <c r="T5" s="13">
         <f>aeo_hdd_projections!X5/aeo_hdd_projections!$F5</f>
         <v>0.88056855607557638</v>
       </c>
-      <c r="U5" s="15">
+      <c r="U5" s="13">
         <f>aeo_hdd_projections!Y5/aeo_hdd_projections!$F5</f>
         <v>0.87675507020280807</v>
       </c>
-      <c r="V5" s="15">
+      <c r="V5" s="13">
         <f>aeo_hdd_projections!Z5/aeo_hdd_projections!$F5</f>
         <v>0.87294158433003988</v>
       </c>
-      <c r="W5" s="15">
+      <c r="W5" s="13">
         <f>aeo_hdd_projections!AA5/aeo_hdd_projections!$F5</f>
         <v>0.86895475819032764</v>
       </c>
-      <c r="X5" s="15">
+      <c r="X5" s="13">
         <f>aeo_hdd_projections!AB5/aeo_hdd_projections!$F5</f>
         <v>0.86514127231755933</v>
       </c>
-      <c r="Y5" s="15">
+      <c r="Y5" s="13">
         <f>aeo_hdd_projections!AC5/aeo_hdd_projections!$F5</f>
         <v>0.86132778644479113</v>
       </c>
-      <c r="Z5" s="15">
+      <c r="Z5" s="13">
         <f>aeo_hdd_projections!AD5/aeo_hdd_projections!$F5</f>
         <v>0.85751430057202294</v>
       </c>
-      <c r="AA5" s="15">
+      <c r="AA5" s="13">
         <f>aeo_hdd_projections!AE5/aeo_hdd_projections!$F5</f>
         <v>0.85352747443231058</v>
       </c>
-      <c r="AB5" s="15">
+      <c r="AB5" s="13">
         <f>aeo_hdd_projections!AF5/aeo_hdd_projections!$F5</f>
         <v>0.84971398855954239</v>
       </c>
-      <c r="AC5" s="15">
+      <c r="AC5" s="13">
         <f>aeo_hdd_projections!AG5/aeo_hdd_projections!$F5</f>
         <v>0.84590050268677419</v>
       </c>
-      <c r="AD5" s="15">
+      <c r="AD5" s="13">
         <f>aeo_hdd_projections!AH5/aeo_hdd_projections!$F5</f>
         <v>0.84208701681400588</v>
       </c>
-      <c r="AE5" s="15">
+      <c r="AE5" s="13">
         <f>aeo_hdd_projections!AI5/aeo_hdd_projections!$F5</f>
         <v>0.83810019067429364</v>
       </c>
-      <c r="AF5" s="15">
+      <c r="AF5" s="13">
         <f>aeo_hdd_projections!AJ5/aeo_hdd_projections!$F5</f>
         <v>0.83428670480152545</v>
       </c>
-      <c r="AG5" s="15">
+      <c r="AG5" s="13">
         <f>aeo_hdd_projections!AK5/aeo_hdd_projections!$F5</f>
         <v>0.83047321892875714</v>
       </c>
-      <c r="AH5" s="15">
+      <c r="AH5" s="13">
         <f>aeo_hdd_projections!AL5/aeo_hdd_projections!$F5</f>
         <v>0.82665973305598894</v>
       </c>
@@ -58779,135 +58786,135 @@
       <c r="A6" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="13">
         <f>aeo_hdd_projections!$F6/aeo_hdd_projections!$F6</f>
         <v>1</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <f>aeo_hdd_projections!G6/aeo_hdd_projections!$F6</f>
         <v>1.1042013311148087</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <f>aeo_hdd_projections!H6/aeo_hdd_projections!$F6</f>
         <v>0.99500831946755408</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <f>aeo_hdd_projections!I6/aeo_hdd_projections!$F6</f>
         <v>0.97628951747088188</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <f>aeo_hdd_projections!J6/aeo_hdd_projections!$F6</f>
         <v>1.03369384359401</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <f>aeo_hdd_projections!K6/aeo_hdd_projections!$F6</f>
         <v>1.0353577371048253</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="13">
         <f>aeo_hdd_projections!L6/aeo_hdd_projections!$F6</f>
         <v>0.99604825291181365</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <f>aeo_hdd_projections!M6/aeo_hdd_projections!$F6</f>
         <v>0.99334442595673877</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="13">
         <f>aeo_hdd_projections!N6/aeo_hdd_projections!$F6</f>
         <v>0.9906405990016639</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="13">
         <f>aeo_hdd_projections!O6/aeo_hdd_projections!$F6</f>
         <v>0.98814475873544094</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="13">
         <f>aeo_hdd_projections!P6/aeo_hdd_projections!$F6</f>
         <v>0.98544093178036607</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="13">
         <f>aeo_hdd_projections!Q6/aeo_hdd_projections!$F6</f>
         <v>0.9827371048252912</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="13">
         <f>aeo_hdd_projections!R6/aeo_hdd_projections!$F6</f>
         <v>0.98003327787021632</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="13">
         <f>aeo_hdd_projections!S6/aeo_hdd_projections!$F6</f>
         <v>0.97712146422628954</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="13">
         <f>aeo_hdd_projections!T6/aeo_hdd_projections!$F6</f>
         <v>0.97441763727121466</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="13">
         <f>aeo_hdd_projections!U6/aeo_hdd_projections!$F6</f>
         <v>0.97171381031613979</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="13">
         <f>aeo_hdd_projections!V6/aeo_hdd_projections!$F6</f>
         <v>0.96880199667221301</v>
       </c>
-      <c r="S6" s="15">
+      <c r="S6" s="13">
         <f>aeo_hdd_projections!W6/aeo_hdd_projections!$F6</f>
         <v>0.96609816971713813</v>
       </c>
-      <c r="T6" s="15">
+      <c r="T6" s="13">
         <f>aeo_hdd_projections!X6/aeo_hdd_projections!$F6</f>
         <v>0.96339434276206326</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U6" s="13">
         <f>aeo_hdd_projections!Y6/aeo_hdd_projections!$F6</f>
         <v>0.96069051580698839</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="13">
         <f>aeo_hdd_projections!Z6/aeo_hdd_projections!$F6</f>
         <v>0.95798668885191351</v>
       </c>
-      <c r="W6" s="15">
+      <c r="W6" s="13">
         <f>aeo_hdd_projections!AA6/aeo_hdd_projections!$F6</f>
         <v>0.95528286189683864</v>
       </c>
-      <c r="X6" s="15">
+      <c r="X6" s="13">
         <f>aeo_hdd_projections!AB6/aeo_hdd_projections!$F6</f>
         <v>0.95257903494176377</v>
       </c>
-      <c r="Y6" s="15">
+      <c r="Y6" s="13">
         <f>aeo_hdd_projections!AC6/aeo_hdd_projections!$F6</f>
         <v>0.95008319467554081</v>
       </c>
-      <c r="Z6" s="15">
+      <c r="Z6" s="13">
         <f>aeo_hdd_projections!AD6/aeo_hdd_projections!$F6</f>
         <v>0.94737936772046594</v>
       </c>
-      <c r="AA6" s="15">
+      <c r="AA6" s="13">
         <f>aeo_hdd_projections!AE6/aeo_hdd_projections!$F6</f>
         <v>0.94467554076539106</v>
       </c>
-      <c r="AB6" s="15">
+      <c r="AB6" s="13">
         <f>aeo_hdd_projections!AF6/aeo_hdd_projections!$F6</f>
         <v>0.9421797004991681</v>
       </c>
-      <c r="AC6" s="15">
+      <c r="AC6" s="13">
         <f>aeo_hdd_projections!AG6/aeo_hdd_projections!$F6</f>
         <v>0.93947587354409323</v>
       </c>
-      <c r="AD6" s="15">
+      <c r="AD6" s="13">
         <f>aeo_hdd_projections!AH6/aeo_hdd_projections!$F6</f>
         <v>0.93677204658901825</v>
       </c>
-      <c r="AE6" s="15">
+      <c r="AE6" s="13">
         <f>aeo_hdd_projections!AI6/aeo_hdd_projections!$F6</f>
         <v>0.93427620632279529</v>
       </c>
-      <c r="AF6" s="15">
+      <c r="AF6" s="13">
         <f>aeo_hdd_projections!AJ6/aeo_hdd_projections!$F6</f>
         <v>0.93157237936772042</v>
       </c>
-      <c r="AG6" s="15">
+      <c r="AG6" s="13">
         <f>aeo_hdd_projections!AK6/aeo_hdd_projections!$F6</f>
         <v>0.92907653910149746</v>
       </c>
-      <c r="AH6" s="15">
+      <c r="AH6" s="13">
         <f>aeo_hdd_projections!AL6/aeo_hdd_projections!$F6</f>
         <v>0.92637271214642258</v>
       </c>
@@ -58916,135 +58923,135 @@
       <c r="A7" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="13">
         <f>aeo_hdd_projections!$F7/aeo_hdd_projections!$F7</f>
         <v>1</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <f>aeo_hdd_projections!G7/aeo_hdd_projections!$F7</f>
         <v>1.0340028467499605</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <f>aeo_hdd_projections!H7/aeo_hdd_projections!$F7</f>
         <v>0.92076545943381305</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <f>aeo_hdd_projections!I7/aeo_hdd_projections!$F7</f>
         <v>0.91712794559544519</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <f>aeo_hdd_projections!J7/aeo_hdd_projections!$F7</f>
         <v>0.98023090305234861</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <f>aeo_hdd_projections!K7/aeo_hdd_projections!$F7</f>
         <v>1.0153408192313775</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="13">
         <f>aeo_hdd_projections!L7/aeo_hdd_projections!$F7</f>
         <v>0.94448837577099476</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="13">
         <f>aeo_hdd_projections!M7/aeo_hdd_projections!$F7</f>
         <v>0.9408508619326269</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="13">
         <f>aeo_hdd_projections!N7/aeo_hdd_projections!$F7</f>
         <v>0.93705519531867787</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="13">
         <f>aeo_hdd_projections!O7/aeo_hdd_projections!$F7</f>
         <v>0.93341768148031001</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="13">
         <f>aeo_hdd_projections!P7/aeo_hdd_projections!$F7</f>
         <v>0.92962201486636087</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="13">
         <f>aeo_hdd_projections!Q7/aeo_hdd_projections!$F7</f>
         <v>0.92582634825241183</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="13">
         <f>aeo_hdd_projections!R7/aeo_hdd_projections!$F7</f>
         <v>0.9220306816384628</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="13">
         <f>aeo_hdd_projections!S7/aeo_hdd_projections!$F7</f>
         <v>0.91839316780009495</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="13">
         <f>aeo_hdd_projections!T7/aeo_hdd_projections!$F7</f>
         <v>0.9145975011861458</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="13">
         <f>aeo_hdd_projections!U7/aeo_hdd_projections!$F7</f>
         <v>0.91080183457219677</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="13">
         <f>aeo_hdd_projections!V7/aeo_hdd_projections!$F7</f>
         <v>0.90700616795824762</v>
       </c>
-      <c r="S7" s="15">
+      <c r="S7" s="13">
         <f>aeo_hdd_projections!W7/aeo_hdd_projections!$F7</f>
         <v>0.90321050134429859</v>
       </c>
-      <c r="T7" s="15">
+      <c r="T7" s="13">
         <f>aeo_hdd_projections!X7/aeo_hdd_projections!$F7</f>
         <v>0.89941483473034955</v>
       </c>
-      <c r="U7" s="15">
+      <c r="U7" s="13">
         <f>aeo_hdd_projections!Y7/aeo_hdd_projections!$F7</f>
         <v>0.89561916811640041</v>
       </c>
-      <c r="V7" s="15">
+      <c r="V7" s="13">
         <f>aeo_hdd_projections!Z7/aeo_hdd_projections!$F7</f>
         <v>0.89182350150245138</v>
       </c>
-      <c r="W7" s="15">
+      <c r="W7" s="13">
         <f>aeo_hdd_projections!AA7/aeo_hdd_projections!$F7</f>
         <v>0.88802783488850234</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="13">
         <f>aeo_hdd_projections!AB7/aeo_hdd_projections!$F7</f>
         <v>0.8842321682745532</v>
       </c>
-      <c r="Y7" s="15">
+      <c r="Y7" s="13">
         <f>aeo_hdd_projections!AC7/aeo_hdd_projections!$F7</f>
         <v>0.88043650166060416</v>
       </c>
-      <c r="Z7" s="15">
+      <c r="Z7" s="13">
         <f>aeo_hdd_projections!AD7/aeo_hdd_projections!$F7</f>
         <v>0.87664083504665502</v>
       </c>
-      <c r="AA7" s="15">
+      <c r="AA7" s="13">
         <f>aeo_hdd_projections!AE7/aeo_hdd_projections!$F7</f>
         <v>0.87284516843270599</v>
       </c>
-      <c r="AB7" s="15">
+      <c r="AB7" s="13">
         <f>aeo_hdd_projections!AF7/aeo_hdd_projections!$F7</f>
         <v>0.86904950181875695</v>
       </c>
-      <c r="AC7" s="15">
+      <c r="AC7" s="13">
         <f>aeo_hdd_projections!AG7/aeo_hdd_projections!$F7</f>
         <v>0.86525383520480781</v>
       </c>
-      <c r="AD7" s="15">
+      <c r="AD7" s="13">
         <f>aeo_hdd_projections!AH7/aeo_hdd_projections!$F7</f>
         <v>0.86145816859085877</v>
       </c>
-      <c r="AE7" s="15">
+      <c r="AE7" s="13">
         <f>aeo_hdd_projections!AI7/aeo_hdd_projections!$F7</f>
         <v>0.85766250197690974</v>
       </c>
-      <c r="AF7" s="15">
+      <c r="AF7" s="13">
         <f>aeo_hdd_projections!AJ7/aeo_hdd_projections!$F7</f>
         <v>0.8538668353629606</v>
       </c>
-      <c r="AG7" s="15">
+      <c r="AG7" s="13">
         <f>aeo_hdd_projections!AK7/aeo_hdd_projections!$F7</f>
         <v>0.84991301597343039</v>
       </c>
-      <c r="AH7" s="15">
+      <c r="AH7" s="13">
         <f>aeo_hdd_projections!AL7/aeo_hdd_projections!$F7</f>
         <v>0.84611734935948124</v>
       </c>
@@ -59053,135 +59060,135 @@
       <c r="A8" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="13">
         <f>aeo_hdd_projections!$F8/aeo_hdd_projections!$F8</f>
         <v>1</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="13">
         <f>aeo_hdd_projections!G8/aeo_hdd_projections!$F8</f>
         <v>1.1182219419924337</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <f>aeo_hdd_projections!H8/aeo_hdd_projections!$F8</f>
         <v>1.0148171500630516</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <f>aeo_hdd_projections!I8/aeo_hdd_projections!$F8</f>
         <v>1.0523329129886507</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <f>aeo_hdd_projections!J8/aeo_hdd_projections!$F8</f>
         <v>1.0126103404791928</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <f>aeo_hdd_projections!K8/aeo_hdd_projections!$F8</f>
         <v>1.1043505674653216</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="13">
         <f>aeo_hdd_projections!L8/aeo_hdd_projections!$F8</f>
         <v>1.0245901639344261</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="13">
         <f>aeo_hdd_projections!M8/aeo_hdd_projections!$F8</f>
         <v>1.0217528373266078</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="13">
         <f>aeo_hdd_projections!N8/aeo_hdd_projections!$F8</f>
         <v>1.0189155107187895</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="13">
         <f>aeo_hdd_projections!O8/aeo_hdd_projections!$F8</f>
         <v>1.016078184110971</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="13">
         <f>aeo_hdd_projections!P8/aeo_hdd_projections!$F8</f>
         <v>1.0129255989911727</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="13">
         <f>aeo_hdd_projections!Q8/aeo_hdd_projections!$F8</f>
         <v>1.0100882723833544</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="13">
         <f>aeo_hdd_projections!R8/aeo_hdd_projections!$F8</f>
         <v>1.0072509457755359</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="13">
         <f>aeo_hdd_projections!S8/aeo_hdd_projections!$F8</f>
         <v>1.0040983606557377</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="13">
         <f>aeo_hdd_projections!T8/aeo_hdd_projections!$F8</f>
         <v>1.0012610340479193</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="13">
         <f>aeo_hdd_projections!U8/aeo_hdd_projections!$F8</f>
         <v>0.99810844892812101</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="13">
         <f>aeo_hdd_projections!V8/aeo_hdd_projections!$F8</f>
         <v>0.99527112232030268</v>
       </c>
-      <c r="S8" s="15">
+      <c r="S8" s="13">
         <f>aeo_hdd_projections!W8/aeo_hdd_projections!$F8</f>
         <v>0.99211853720050447</v>
       </c>
-      <c r="T8" s="15">
+      <c r="T8" s="13">
         <f>aeo_hdd_projections!X8/aeo_hdd_projections!$F8</f>
         <v>0.98896595208070615</v>
       </c>
-      <c r="U8" s="15">
+      <c r="U8" s="13">
         <f>aeo_hdd_projections!Y8/aeo_hdd_projections!$F8</f>
         <v>0.98612862547288782</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="13">
         <f>aeo_hdd_projections!Z8/aeo_hdd_projections!$F8</f>
         <v>0.9829760403530895</v>
       </c>
-      <c r="W8" s="15">
+      <c r="W8" s="13">
         <f>aeo_hdd_projections!AA8/aeo_hdd_projections!$F8</f>
         <v>0.97982345523329129</v>
       </c>
-      <c r="X8" s="15">
+      <c r="X8" s="13">
         <f>aeo_hdd_projections!AB8/aeo_hdd_projections!$F8</f>
         <v>0.97667087011349307</v>
       </c>
-      <c r="Y8" s="15">
+      <c r="Y8" s="13">
         <f>aeo_hdd_projections!AC8/aeo_hdd_projections!$F8</f>
         <v>0.97383354350567464</v>
       </c>
-      <c r="Z8" s="15">
+      <c r="Z8" s="13">
         <f>aeo_hdd_projections!AD8/aeo_hdd_projections!$F8</f>
         <v>0.97068095838587642</v>
       </c>
-      <c r="AA8" s="15">
+      <c r="AA8" s="13">
         <f>aeo_hdd_projections!AE8/aeo_hdd_projections!$F8</f>
         <v>0.96752837326607821</v>
       </c>
-      <c r="AB8" s="15">
+      <c r="AB8" s="13">
         <f>aeo_hdd_projections!AF8/aeo_hdd_projections!$F8</f>
         <v>0.96437578814628</v>
       </c>
-      <c r="AC8" s="15">
+      <c r="AC8" s="13">
         <f>aeo_hdd_projections!AG8/aeo_hdd_projections!$F8</f>
         <v>0.96122320302648168</v>
       </c>
-      <c r="AD8" s="15">
+      <c r="AD8" s="13">
         <f>aeo_hdd_projections!AH8/aeo_hdd_projections!$F8</f>
         <v>0.95838587641866335</v>
       </c>
-      <c r="AE8" s="15">
+      <c r="AE8" s="13">
         <f>aeo_hdd_projections!AI8/aeo_hdd_projections!$F8</f>
         <v>0.95523329129886503</v>
       </c>
-      <c r="AF8" s="15">
+      <c r="AF8" s="13">
         <f>aeo_hdd_projections!AJ8/aeo_hdd_projections!$F8</f>
         <v>0.95208070617906682</v>
       </c>
-      <c r="AG8" s="15">
+      <c r="AG8" s="13">
         <f>aeo_hdd_projections!AK8/aeo_hdd_projections!$F8</f>
         <v>0.9489281210592686</v>
       </c>
-      <c r="AH8" s="15">
+      <c r="AH8" s="13">
         <f>aeo_hdd_projections!AL8/aeo_hdd_projections!$F8</f>
         <v>0.94577553593947039</v>
       </c>
@@ -59190,135 +59197,135 @@
       <c r="A9" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="13">
         <f>aeo_hdd_projections!$F9/aeo_hdd_projections!$F9</f>
         <v>1</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="13">
         <f>aeo_hdd_projections!G9/aeo_hdd_projections!$F9</f>
         <v>0.90674753601213043</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="13">
         <f>aeo_hdd_projections!H9/aeo_hdd_projections!$F9</f>
         <v>0.85784685367702807</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="13">
         <f>aeo_hdd_projections!I9/aeo_hdd_projections!$F9</f>
         <v>0.89689158453373763</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="13">
         <f>aeo_hdd_projections!J9/aeo_hdd_projections!$F9</f>
         <v>0.9727065959059894</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <f>aeo_hdd_projections!K9/aeo_hdd_projections!$F9</f>
         <v>0.98559514783927216</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="13">
         <f>aeo_hdd_projections!L9/aeo_hdd_projections!$F9</f>
         <v>0.900303260045489</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <f>aeo_hdd_projections!M9/aeo_hdd_projections!$F9</f>
         <v>0.89385898407884756</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="13">
         <f>aeo_hdd_projections!N9/aeo_hdd_projections!$F9</f>
         <v>0.88779378316906743</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="13">
         <f>aeo_hdd_projections!O9/aeo_hdd_projections!$F9</f>
         <v>0.8817285822592873</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="13">
         <f>aeo_hdd_projections!P9/aeo_hdd_projections!$F9</f>
         <v>0.87566338134950716</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="13">
         <f>aeo_hdd_projections!Q9/aeo_hdd_projections!$F9</f>
         <v>0.86959818043972703</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="13">
         <f>aeo_hdd_projections!R9/aeo_hdd_projections!$F9</f>
         <v>0.86315390447308571</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="13">
         <f>aeo_hdd_projections!S9/aeo_hdd_projections!$F9</f>
         <v>0.85708870356330558</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="13">
         <f>aeo_hdd_projections!T9/aeo_hdd_projections!$F9</f>
         <v>0.85102350265352544</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="Q9" s="13">
         <f>aeo_hdd_projections!U9/aeo_hdd_projections!$F9</f>
         <v>0.84495830174374531</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="13">
         <f>aeo_hdd_projections!V9/aeo_hdd_projections!$F9</f>
         <v>0.83889310083396518</v>
       </c>
-      <c r="S9" s="15">
+      <c r="S9" s="13">
         <f>aeo_hdd_projections!W9/aeo_hdd_projections!$F9</f>
         <v>0.83282789992418493</v>
       </c>
-      <c r="T9" s="15">
+      <c r="T9" s="13">
         <f>aeo_hdd_projections!X9/aeo_hdd_projections!$F9</f>
         <v>0.82638362395754361</v>
       </c>
-      <c r="U9" s="15">
+      <c r="U9" s="13">
         <f>aeo_hdd_projections!Y9/aeo_hdd_projections!$F9</f>
         <v>0.82031842304776348</v>
       </c>
-      <c r="V9" s="15">
+      <c r="V9" s="13">
         <f>aeo_hdd_projections!Z9/aeo_hdd_projections!$F9</f>
         <v>0.81425322213798335</v>
       </c>
-      <c r="W9" s="15">
+      <c r="W9" s="13">
         <f>aeo_hdd_projections!AA9/aeo_hdd_projections!$F9</f>
         <v>0.80818802122820321</v>
       </c>
-      <c r="X9" s="15">
+      <c r="X9" s="13">
         <f>aeo_hdd_projections!AB9/aeo_hdd_projections!$F9</f>
         <v>0.80212282031842308</v>
       </c>
-      <c r="Y9" s="15">
+      <c r="Y9" s="13">
         <f>aeo_hdd_projections!AC9/aeo_hdd_projections!$F9</f>
         <v>0.79605761940864295</v>
       </c>
-      <c r="Z9" s="15">
+      <c r="Z9" s="13">
         <f>aeo_hdd_projections!AD9/aeo_hdd_projections!$F9</f>
         <v>0.78999241849886281</v>
       </c>
-      <c r="AA9" s="15">
+      <c r="AA9" s="13">
         <f>aeo_hdd_projections!AE9/aeo_hdd_projections!$F9</f>
         <v>0.78392721758908268</v>
       </c>
-      <c r="AB9" s="15">
+      <c r="AB9" s="13">
         <f>aeo_hdd_projections!AF9/aeo_hdd_projections!$F9</f>
         <v>0.77786201667930255</v>
       </c>
-      <c r="AC9" s="15">
+      <c r="AC9" s="13">
         <f>aeo_hdd_projections!AG9/aeo_hdd_projections!$F9</f>
         <v>0.77179681576952242</v>
       </c>
-      <c r="AD9" s="15">
+      <c r="AD9" s="13">
         <f>aeo_hdd_projections!AH9/aeo_hdd_projections!$F9</f>
         <v>0.76573161485974228</v>
       </c>
-      <c r="AE9" s="15">
+      <c r="AE9" s="13">
         <f>aeo_hdd_projections!AI9/aeo_hdd_projections!$F9</f>
         <v>0.76004548900682334</v>
       </c>
-      <c r="AF9" s="15">
+      <c r="AF9" s="13">
         <f>aeo_hdd_projections!AJ9/aeo_hdd_projections!$F9</f>
         <v>0.75398028809704321</v>
       </c>
-      <c r="AG9" s="15">
+      <c r="AG9" s="13">
         <f>aeo_hdd_projections!AK9/aeo_hdd_projections!$F9</f>
         <v>0.74791508718726307</v>
       </c>
-      <c r="AH9" s="15">
+      <c r="AH9" s="13">
         <f>aeo_hdd_projections!AL9/aeo_hdd_projections!$F9</f>
         <v>0.74184988627748294</v>
       </c>
@@ -59327,135 +59334,135 @@
       <c r="A10" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="13">
         <f>aeo_hdd_projections!$F10/aeo_hdd_projections!$F10</f>
         <v>1</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <f>aeo_hdd_projections!G10/aeo_hdd_projections!$F10</f>
         <v>1.0154860911958703</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <f>aeo_hdd_projections!H10/aeo_hdd_projections!$F10</f>
         <v>0.90708345282477776</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <f>aeo_hdd_projections!I10/aeo_hdd_projections!$F10</f>
         <v>0.86908517350157732</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <f>aeo_hdd_projections!J10/aeo_hdd_projections!$F10</f>
         <v>0.98150272440493258</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <f>aeo_hdd_projections!K10/aeo_hdd_projections!$F10</f>
         <v>0.94651562948092915</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="13">
         <f>aeo_hdd_projections!L10/aeo_hdd_projections!$F10</f>
         <v>0.91038141669056494</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="13">
         <f>aeo_hdd_projections!M10/aeo_hdd_projections!$F10</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="13">
         <f>aeo_hdd_projections!N10/aeo_hdd_projections!$F10</f>
         <v>0.9076570117579581</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="13">
         <f>aeo_hdd_projections!O10/aeo_hdd_projections!$F10</f>
         <v>0.90636650415830222</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="13">
         <f>aeo_hdd_projections!P10/aeo_hdd_projections!$F10</f>
         <v>0.90493260682535126</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="13">
         <f>aeo_hdd_projections!Q10/aeo_hdd_projections!$F10</f>
         <v>0.9034987094924003</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="13">
         <f>aeo_hdd_projections!R10/aeo_hdd_projections!$F10</f>
         <v>0.90206481215944934</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="13">
         <f>aeo_hdd_projections!S10/aeo_hdd_projections!$F10</f>
         <v>0.90063091482649837</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="13">
         <f>aeo_hdd_projections!T10/aeo_hdd_projections!$F10</f>
         <v>0.89919701749354741</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="Q10" s="13">
         <f>aeo_hdd_projections!U10/aeo_hdd_projections!$F10</f>
         <v>0.89776312016059645</v>
       </c>
-      <c r="R10" s="15">
+      <c r="R10" s="13">
         <f>aeo_hdd_projections!V10/aeo_hdd_projections!$F10</f>
         <v>0.8961858330943504</v>
       </c>
-      <c r="S10" s="15">
+      <c r="S10" s="13">
         <f>aeo_hdd_projections!W10/aeo_hdd_projections!$F10</f>
         <v>0.89475193576139944</v>
       </c>
-      <c r="T10" s="15">
+      <c r="T10" s="13">
         <f>aeo_hdd_projections!X10/aeo_hdd_projections!$F10</f>
         <v>0.89331803842844848</v>
       </c>
-      <c r="U10" s="15">
+      <c r="U10" s="13">
         <f>aeo_hdd_projections!Y10/aeo_hdd_projections!$F10</f>
         <v>0.89174075136220243</v>
       </c>
-      <c r="V10" s="15">
+      <c r="V10" s="13">
         <f>aeo_hdd_projections!Z10/aeo_hdd_projections!$F10</f>
         <v>0.89030685402925147</v>
       </c>
-      <c r="W10" s="15">
+      <c r="W10" s="13">
         <f>aeo_hdd_projections!AA10/aeo_hdd_projections!$F10</f>
         <v>0.88872956696300542</v>
       </c>
-      <c r="X10" s="15">
+      <c r="X10" s="13">
         <f>aeo_hdd_projections!AB10/aeo_hdd_projections!$F10</f>
         <v>0.88729566963005446</v>
       </c>
-      <c r="Y10" s="15">
+      <c r="Y10" s="13">
         <f>aeo_hdd_projections!AC10/aeo_hdd_projections!$F10</f>
         <v>0.88571838256380842</v>
       </c>
-      <c r="Z10" s="15">
+      <c r="Z10" s="13">
         <f>aeo_hdd_projections!AD10/aeo_hdd_projections!$F10</f>
         <v>0.88428448523085745</v>
       </c>
-      <c r="AA10" s="15">
+      <c r="AA10" s="13">
         <f>aeo_hdd_projections!AE10/aeo_hdd_projections!$F10</f>
         <v>0.88270719816461141</v>
       </c>
-      <c r="AB10" s="15">
+      <c r="AB10" s="13">
         <f>aeo_hdd_projections!AF10/aeo_hdd_projections!$F10</f>
         <v>0.88112991109836536</v>
       </c>
-      <c r="AC10" s="15">
+      <c r="AC10" s="13">
         <f>aeo_hdd_projections!AG10/aeo_hdd_projections!$F10</f>
         <v>0.8796960137654144</v>
       </c>
-      <c r="AD10" s="15">
+      <c r="AD10" s="13">
         <f>aeo_hdd_projections!AH10/aeo_hdd_projections!$F10</f>
         <v>0.87811872669916835</v>
       </c>
-      <c r="AE10" s="15">
+      <c r="AE10" s="13">
         <f>aeo_hdd_projections!AI10/aeo_hdd_projections!$F10</f>
         <v>0.8765414396329223</v>
       </c>
-      <c r="AF10" s="15">
+      <c r="AF10" s="13">
         <f>aeo_hdd_projections!AJ10/aeo_hdd_projections!$F10</f>
         <v>0.87510754229997134</v>
       </c>
-      <c r="AG10" s="15">
+      <c r="AG10" s="13">
         <f>aeo_hdd_projections!AK10/aeo_hdd_projections!$F10</f>
         <v>0.87353025523372529</v>
       </c>
-      <c r="AH10" s="15">
+      <c r="AH10" s="13">
         <f>aeo_hdd_projections!AL10/aeo_hdd_projections!$F10</f>
         <v>0.87195296816747925</v>
       </c>
@@ -59464,135 +59471,135 @@
       <c r="A11" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="13">
         <f>aeo_hdd_projections!$F11/aeo_hdd_projections!$F11</f>
         <v>1</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <f>aeo_hdd_projections!G11/aeo_hdd_projections!$F11</f>
         <v>0.95159857904085254</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="13">
         <f>aeo_hdd_projections!H11/aeo_hdd_projections!$F11</f>
         <v>0.80461811722912968</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <f>aeo_hdd_projections!I11/aeo_hdd_projections!$F11</f>
         <v>0.84857904085257552</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="13">
         <f>aeo_hdd_projections!J11/aeo_hdd_projections!$F11</f>
         <v>0.97468916518650084</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <f>aeo_hdd_projections!K11/aeo_hdd_projections!$F11</f>
         <v>0.91296625222024863</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <f>aeo_hdd_projections!L11/aeo_hdd_projections!$F11</f>
         <v>0.86234458259325042</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <f>aeo_hdd_projections!M11/aeo_hdd_projections!$F11</f>
         <v>0.85879218472468921</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="13">
         <f>aeo_hdd_projections!N11/aeo_hdd_projections!$F11</f>
         <v>0.85479573712255774</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="13">
         <f>aeo_hdd_projections!O11/aeo_hdd_projections!$F11</f>
         <v>0.85079928952042627</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="13">
         <f>aeo_hdd_projections!P11/aeo_hdd_projections!$F11</f>
         <v>0.84724689165186506</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="13">
         <f>aeo_hdd_projections!Q11/aeo_hdd_projections!$F11</f>
         <v>0.84325044404973359</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="13">
         <f>aeo_hdd_projections!R11/aeo_hdd_projections!$F11</f>
         <v>0.83969804618117228</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="13">
         <f>aeo_hdd_projections!S11/aeo_hdd_projections!$F11</f>
         <v>0.83570159857904081</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="13">
         <f>aeo_hdd_projections!T11/aeo_hdd_projections!$F11</f>
         <v>0.8321492007104796</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="13">
         <f>aeo_hdd_projections!U11/aeo_hdd_projections!$F11</f>
         <v>0.82815275310834813</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="13">
         <f>aeo_hdd_projections!V11/aeo_hdd_projections!$F11</f>
         <v>0.82460035523978681</v>
       </c>
-      <c r="S11" s="15">
+      <c r="S11" s="13">
         <f>aeo_hdd_projections!W11/aeo_hdd_projections!$F11</f>
         <v>0.8210479573712256</v>
       </c>
-      <c r="T11" s="15">
+      <c r="T11" s="13">
         <f>aeo_hdd_projections!X11/aeo_hdd_projections!$F11</f>
         <v>0.81705150976909413</v>
       </c>
-      <c r="U11" s="15">
+      <c r="U11" s="13">
         <f>aeo_hdd_projections!Y11/aeo_hdd_projections!$F11</f>
         <v>0.81349911190053281</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="13">
         <f>aeo_hdd_projections!Z11/aeo_hdd_projections!$F11</f>
         <v>0.8099467140319716</v>
       </c>
-      <c r="W11" s="15">
+      <c r="W11" s="13">
         <f>aeo_hdd_projections!AA11/aeo_hdd_projections!$F11</f>
         <v>0.80595026642984013</v>
       </c>
-      <c r="X11" s="15">
+      <c r="X11" s="13">
         <f>aeo_hdd_projections!AB11/aeo_hdd_projections!$F11</f>
         <v>0.80239786856127882</v>
       </c>
-      <c r="Y11" s="15">
+      <c r="Y11" s="13">
         <f>aeo_hdd_projections!AC11/aeo_hdd_projections!$F11</f>
         <v>0.79884547069271761</v>
       </c>
-      <c r="Z11" s="15">
+      <c r="Z11" s="13">
         <f>aeo_hdd_projections!AD11/aeo_hdd_projections!$F11</f>
         <v>0.79529307282415629</v>
       </c>
-      <c r="AA11" s="15">
+      <c r="AA11" s="13">
         <f>aeo_hdd_projections!AE11/aeo_hdd_projections!$F11</f>
         <v>0.79174067495559508</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AB11" s="13">
         <f>aeo_hdd_projections!AF11/aeo_hdd_projections!$F11</f>
         <v>0.78774422735346361</v>
       </c>
-      <c r="AC11" s="15">
+      <c r="AC11" s="13">
         <f>aeo_hdd_projections!AG11/aeo_hdd_projections!$F11</f>
         <v>0.78419182948490229</v>
       </c>
-      <c r="AD11" s="15">
+      <c r="AD11" s="13">
         <f>aeo_hdd_projections!AH11/aeo_hdd_projections!$F11</f>
         <v>0.78063943161634108</v>
       </c>
-      <c r="AE11" s="15">
+      <c r="AE11" s="13">
         <f>aeo_hdd_projections!AI11/aeo_hdd_projections!$F11</f>
         <v>0.77708703374777977</v>
       </c>
-      <c r="AF11" s="15">
+      <c r="AF11" s="13">
         <f>aeo_hdd_projections!AJ11/aeo_hdd_projections!$F11</f>
         <v>0.77353463587921845</v>
       </c>
-      <c r="AG11" s="15">
+      <c r="AG11" s="13">
         <f>aeo_hdd_projections!AK11/aeo_hdd_projections!$F11</f>
         <v>0.76998223801065724</v>
       </c>
-      <c r="AH11" s="15">
+      <c r="AH11" s="13">
         <f>aeo_hdd_projections!AL11/aeo_hdd_projections!$F11</f>
         <v>0.76642984014209592</v>
       </c>
@@ -59638,7 +59645,7 @@
   <dimension ref="A1:AL11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59648,125 +59655,125 @@
     <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>415</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="D1" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="J1" s="12">
+      <c r="F1" s="14">
+        <v>2018</v>
+      </c>
+      <c r="G1" s="14">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="14">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="14">
+        <v>2021</v>
+      </c>
+      <c r="J1" s="14">
         <v>2022</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="14">
         <v>2023</v>
       </c>
-      <c r="L1" s="12">
+      <c r="L1" s="14">
         <v>2024</v>
       </c>
-      <c r="M1" s="12">
+      <c r="M1" s="14">
         <v>2025</v>
       </c>
-      <c r="N1" s="12">
+      <c r="N1" s="14">
         <v>2026</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="14">
         <v>2027</v>
       </c>
-      <c r="P1" s="12">
+      <c r="P1" s="14">
         <v>2028</v>
       </c>
-      <c r="Q1" s="12">
+      <c r="Q1" s="14">
         <v>2029</v>
       </c>
-      <c r="R1" s="12">
+      <c r="R1" s="14">
         <v>2030</v>
       </c>
-      <c r="S1" s="12">
+      <c r="S1" s="14">
         <v>2031</v>
       </c>
-      <c r="T1" s="12">
+      <c r="T1" s="14">
         <v>2032</v>
       </c>
-      <c r="U1" s="12">
+      <c r="U1" s="14">
         <v>2033</v>
       </c>
-      <c r="V1" s="12">
+      <c r="V1" s="14">
         <v>2034</v>
       </c>
-      <c r="W1" s="12">
+      <c r="W1" s="14">
         <v>2035</v>
       </c>
-      <c r="X1" s="12">
+      <c r="X1" s="14">
         <v>2036</v>
       </c>
-      <c r="Y1" s="12">
+      <c r="Y1" s="14">
         <v>2037</v>
       </c>
-      <c r="Z1" s="12">
+      <c r="Z1" s="14">
         <v>2038</v>
       </c>
-      <c r="AA1" s="12">
+      <c r="AA1" s="14">
         <v>2039</v>
       </c>
-      <c r="AB1" s="12">
+      <c r="AB1" s="14">
         <v>2040</v>
       </c>
-      <c r="AC1" s="12">
+      <c r="AC1" s="14">
         <v>2041</v>
       </c>
-      <c r="AD1" s="12">
+      <c r="AD1" s="14">
         <v>2042</v>
       </c>
-      <c r="AE1" s="12">
+      <c r="AE1" s="14">
         <v>2043</v>
       </c>
-      <c r="AF1" s="12">
+      <c r="AF1" s="14">
         <v>2044</v>
       </c>
-      <c r="AG1" s="12">
+      <c r="AG1" s="14">
         <v>2045</v>
       </c>
-      <c r="AH1" s="12">
+      <c r="AH1" s="14">
         <v>2046</v>
       </c>
-      <c r="AI1" s="12">
+      <c r="AI1" s="14">
         <v>2047</v>
       </c>
-      <c r="AJ1" s="12">
+      <c r="AJ1" s="14">
         <v>2048</v>
       </c>
-      <c r="AK1" s="12">
+      <c r="AK1" s="14">
         <v>2049</v>
       </c>
-      <c r="AL1" s="12">
+      <c r="AL1" s="14">
         <v>2050</v>
       </c>
     </row>
     <row r="2" spans="1:38" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>409</v>
@@ -59778,18 +59785,18 @@
         <v>411</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" s="14">
+        <v>413</v>
+      </c>
+      <c r="F2" s="12">
         <v>4291</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="12">
         <v>4317</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="12">
         <v>3914</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="12">
         <v>3934</v>
       </c>
       <c r="J2" s="5">
@@ -59894,18 +59901,18 @@
         <v>411</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F3" s="14">
+        <v>413</v>
+      </c>
+      <c r="F3" s="12">
         <v>6434</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="12">
         <v>6427</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="12">
         <v>5855</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="12">
         <v>5747</v>
       </c>
       <c r="J3" s="5">
@@ -60010,18 +60017,18 @@
         <v>411</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F4" s="14">
+        <v>413</v>
+      </c>
+      <c r="F4" s="12">
         <v>3479</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="12">
         <v>3181</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12">
         <v>3064</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="12">
         <v>3166</v>
       </c>
       <c r="J4" s="5">
@@ -60126,18 +60133,18 @@
         <v>411</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" s="14">
+        <v>413</v>
+      </c>
+      <c r="F5" s="12">
         <v>5769</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>5736</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>5199</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <v>5262</v>
       </c>
       <c r="J5" s="5">
@@ -60242,18 +60249,18 @@
         <v>411</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F6" s="14">
+        <v>413</v>
+      </c>
+      <c r="F6" s="12">
         <v>4808</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>5309</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>4784</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="12">
         <v>4694</v>
       </c>
       <c r="J6" s="5">
@@ -60358,18 +60365,18 @@
         <v>411</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F7" s="14">
+        <v>413</v>
+      </c>
+      <c r="F7" s="12">
         <v>6323</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>6538</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>5822</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="12">
         <v>5799</v>
       </c>
       <c r="J7" s="5">
@@ -60474,18 +60481,18 @@
         <v>411</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F8" s="14">
+        <v>413</v>
+      </c>
+      <c r="F8" s="12">
         <v>3172</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>3547</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>3219</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <v>3338</v>
       </c>
       <c r="J8" s="5">
@@ -60590,18 +60597,18 @@
         <v>411</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F9" s="14">
+        <v>413</v>
+      </c>
+      <c r="F9" s="12">
         <v>2638</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>2392</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>2263</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="12">
         <v>2366</v>
       </c>
       <c r="J9" s="5">
@@ -60706,18 +60713,18 @@
         <v>411</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F10" s="14">
+        <v>413</v>
+      </c>
+      <c r="F10" s="12">
         <v>6974</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>7082</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>6326</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="12">
         <v>6061</v>
       </c>
       <c r="J10" s="5">
@@ -60822,18 +60829,18 @@
         <v>411</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="F11" s="14">
+        <v>413</v>
+      </c>
+      <c r="F11" s="12">
         <v>2252</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>2143</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>1812</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="12">
         <v>1911</v>
       </c>
       <c r="J11" s="5">
@@ -60934,10 +60941,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F2A8E9-CD99-41A6-AC11-BBCC1A6899F0}">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A20" sqref="A20"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixed code to include more model scenarios and projectsion for consumption, fuel prices, and electricity grid decarb rates - works well on smaller scale and running fine. - need to do a full US run and see where improvements can be made.
</commit_message>
<xml_diff>
--- a/projections/aeo_projections_2022_2050.xlsx
+++ b/projections/aeo_projections_2022_2050.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08E8F73-101E-459D-8E50-7DB69D87EBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06746B86-2C59-436E-819C-CC796F99097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="865" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
+    <workbookView xWindow="2484" yWindow="3576" windowWidth="17280" windowHeight="9960" tabRatio="865" firstSheet="1" activeTab="3" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="fuel_price_factors_2022_2050" sheetId="9" r:id="rId1"/>
     <sheet name="aeo_fuel_price_projections" sheetId="5" r:id="rId2"/>
     <sheet name="hdd_factors_2018_2050" sheetId="10" r:id="rId3"/>
-    <sheet name="aeo_hdd_projections" sheetId="11" r:id="rId4"/>
-    <sheet name="aeo_justify_2022_projections" sheetId="3" r:id="rId5"/>
-    <sheet name="aeo2019_key_indicators" sheetId="2" r:id="rId6"/>
-    <sheet name="aeo2023_key_indicators" sheetId="1" r:id="rId7"/>
+    <sheet name="hdd_factors_2022_2050" sheetId="12" r:id="rId4"/>
+    <sheet name="aeo_hdd_projections" sheetId="11" r:id="rId5"/>
+    <sheet name="aeo_justify_2022_projections" sheetId="3" r:id="rId6"/>
+    <sheet name="aeo2019_key_indicators" sheetId="2" r:id="rId7"/>
+    <sheet name="aeo2023_key_indicators" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="421">
   <si>
     <t>Table 4.  Residential Sector Key Indicators and Consumption</t>
   </si>
@@ -2210,7 +2211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F5499C-249D-4660-AC39-83320A5A905A}">
   <dimension ref="A1:AG247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -59641,11 +59642,1361 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B2126A-7C3E-492E-A994-6660270B8389}">
+  <dimension ref="A1:AD12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="14">
+        <v>2022</v>
+      </c>
+      <c r="C1" s="14">
+        <v>2023</v>
+      </c>
+      <c r="D1" s="14">
+        <v>2024</v>
+      </c>
+      <c r="E1" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F1" s="14">
+        <v>2026</v>
+      </c>
+      <c r="G1" s="14">
+        <v>2027</v>
+      </c>
+      <c r="H1" s="14">
+        <v>2028</v>
+      </c>
+      <c r="I1" s="14">
+        <v>2029</v>
+      </c>
+      <c r="J1" s="14">
+        <v>2030</v>
+      </c>
+      <c r="K1" s="14">
+        <v>2031</v>
+      </c>
+      <c r="L1" s="14">
+        <v>2032</v>
+      </c>
+      <c r="M1" s="14">
+        <v>2033</v>
+      </c>
+      <c r="N1" s="14">
+        <v>2034</v>
+      </c>
+      <c r="O1" s="14">
+        <v>2035</v>
+      </c>
+      <c r="P1" s="14">
+        <v>2036</v>
+      </c>
+      <c r="Q1" s="14">
+        <v>2037</v>
+      </c>
+      <c r="R1" s="14">
+        <v>2038</v>
+      </c>
+      <c r="S1" s="14">
+        <v>2039</v>
+      </c>
+      <c r="T1" s="14">
+        <v>2040</v>
+      </c>
+      <c r="U1" s="14">
+        <v>2041</v>
+      </c>
+      <c r="V1" s="14">
+        <v>2042</v>
+      </c>
+      <c r="W1" s="14">
+        <v>2043</v>
+      </c>
+      <c r="X1" s="14">
+        <v>2044</v>
+      </c>
+      <c r="Y1" s="14">
+        <v>2045</v>
+      </c>
+      <c r="Z1" s="14">
+        <v>2046</v>
+      </c>
+      <c r="AA1" s="14">
+        <v>2047</v>
+      </c>
+      <c r="AB1" s="14">
+        <v>2048</v>
+      </c>
+      <c r="AC1" s="14">
+        <v>2049</v>
+      </c>
+      <c r="AD1" s="14">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="B2" s="13">
+        <f>aeo_hdd_projections!$J2/aeo_hdd_projections!$J2</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="13">
+        <f>aeo_hdd_projections!K2/aeo_hdd_projections!$J2</f>
+        <v>1.0028349414260749</v>
+      </c>
+      <c r="D2" s="13">
+        <f>aeo_hdd_projections!L2/aeo_hdd_projections!$J2</f>
+        <v>0.93895362669639648</v>
+      </c>
+      <c r="E2" s="13">
+        <f>aeo_hdd_projections!M2/aeo_hdd_projections!$J2</f>
+        <v>0.93448443681795335</v>
+      </c>
+      <c r="F2" s="13">
+        <f>aeo_hdd_projections!N2/aeo_hdd_projections!$J2</f>
+        <v>0.93008281697435657</v>
+      </c>
+      <c r="G2" s="13">
+        <f>aeo_hdd_projections!O2/aeo_hdd_projections!$J2</f>
+        <v>0.92570702593261533</v>
+      </c>
+      <c r="H2" s="13">
+        <f>aeo_hdd_projections!P2/aeo_hdd_projections!$J2</f>
+        <v>0.92127790535192067</v>
+      </c>
+      <c r="I2" s="13">
+        <f>aeo_hdd_projections!Q2/aeo_hdd_projections!$J2</f>
+        <v>0.91685385819732035</v>
+      </c>
+      <c r="J2" s="13">
+        <f>aeo_hdd_projections!R2/aeo_hdd_projections!$J2</f>
+        <v>0.91243511518643183</v>
+      </c>
+      <c r="K2" s="13">
+        <f>aeo_hdd_projections!S2/aeo_hdd_projections!$J2</f>
+        <v>0.90803770399112449</v>
+      </c>
+      <c r="L2" s="13">
+        <f>aeo_hdd_projections!T2/aeo_hdd_projections!$J2</f>
+        <v>0.90365412971299153</v>
+      </c>
+      <c r="M2" s="13">
+        <f>aeo_hdd_projections!U2/aeo_hdd_projections!$J2</f>
+        <v>0.89924928123964432</v>
+      </c>
+      <c r="N2" s="13">
+        <f>aeo_hdd_projections!V2/aeo_hdd_projections!$J2</f>
+        <v>0.89487550785534797</v>
+      </c>
+      <c r="O2" s="13">
+        <f>aeo_hdd_projections!W2/aeo_hdd_projections!$J2</f>
+        <v>0.89047584828497828</v>
+      </c>
+      <c r="P2" s="13">
+        <f>aeo_hdd_projections!X2/aeo_hdd_projections!$J2</f>
+        <v>0.88603900208825892</v>
+      </c>
+      <c r="Q2" s="13">
+        <f>aeo_hdd_projections!Y2/aeo_hdd_projections!$J2</f>
+        <v>0.88172859009051963</v>
+      </c>
+      <c r="R2" s="13">
+        <f>aeo_hdd_projections!Z2/aeo_hdd_projections!$J2</f>
+        <v>0.87736588642888202</v>
+      </c>
+      <c r="S2" s="13">
+        <f>aeo_hdd_projections!AA2/aeo_hdd_projections!$J2</f>
+        <v>0.87293140408410852</v>
+      </c>
+      <c r="T2" s="13">
+        <f>aeo_hdd_projections!AB2/aeo_hdd_projections!$J2</f>
+        <v>0.86858392093690284</v>
+      </c>
+      <c r="U2" s="13">
+        <f>aeo_hdd_projections!AC2/aeo_hdd_projections!$J2</f>
+        <v>0.86427022268904585</v>
+      </c>
+      <c r="V2" s="13">
+        <f>aeo_hdd_projections!AD2/aeo_hdd_projections!$J2</f>
+        <v>0.85991207363404953</v>
+      </c>
+      <c r="W2" s="13">
+        <f>aeo_hdd_projections!AE2/aeo_hdd_projections!$J2</f>
+        <v>0.85554418106943442</v>
+      </c>
+      <c r="X2" s="13">
+        <f>aeo_hdd_projections!AF2/aeo_hdd_projections!$J2</f>
+        <v>0.8511753084862802</v>
+      </c>
+      <c r="Y2" s="13">
+        <f>aeo_hdd_projections!AG2/aeo_hdd_projections!$J2</f>
+        <v>0.84682327049628425</v>
+      </c>
+      <c r="Z2" s="13">
+        <f>aeo_hdd_projections!AH2/aeo_hdd_projections!$J2</f>
+        <v>0.84250905342897431</v>
+      </c>
+      <c r="AA2" s="13">
+        <f>aeo_hdd_projections!AI2/aeo_hdd_projections!$J2</f>
+        <v>0.83822475857107515</v>
+      </c>
+      <c r="AB2" s="13">
+        <f>aeo_hdd_projections!AJ2/aeo_hdd_projections!$J2</f>
+        <v>0.83393890725481679</v>
+      </c>
+      <c r="AC2" s="13">
+        <f>aeo_hdd_projections!AK2/aeo_hdd_projections!$J2</f>
+        <v>0.82970552046355817</v>
+      </c>
+      <c r="AD2" s="13">
+        <f>aeo_hdd_projections!AL2/aeo_hdd_projections!$J2</f>
+        <v>0.82550026870573379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="13">
+        <f>aeo_hdd_projections!$J3/aeo_hdd_projections!$J3</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <f>aeo_hdd_projections!K3/aeo_hdd_projections!$J3</f>
+        <v>0.9811731756651626</v>
+      </c>
+      <c r="D3" s="13">
+        <f>aeo_hdd_projections!L3/aeo_hdd_projections!$J3</f>
+        <v>0.93076085265287067</v>
+      </c>
+      <c r="E3" s="13">
+        <f>aeo_hdd_projections!M3/aeo_hdd_projections!$J3</f>
+        <v>0.928426948809709</v>
+      </c>
+      <c r="F3" s="13">
+        <f>aeo_hdd_projections!N3/aeo_hdd_projections!$J3</f>
+        <v>0.92624863855609152</v>
+      </c>
+      <c r="G3" s="13">
+        <f>aeo_hdd_projections!O3/aeo_hdd_projections!$J3</f>
+        <v>0.92391473471292984</v>
+      </c>
+      <c r="H3" s="13">
+        <f>aeo_hdd_projections!P3/aeo_hdd_projections!$J3</f>
+        <v>0.92158083086976816</v>
+      </c>
+      <c r="I3" s="13">
+        <f>aeo_hdd_projections!Q3/aeo_hdd_projections!$J3</f>
+        <v>0.91924692702660649</v>
+      </c>
+      <c r="J3" s="13">
+        <f>aeo_hdd_projections!R3/aeo_hdd_projections!$J3</f>
+        <v>0.91691302318344481</v>
+      </c>
+      <c r="K3" s="13">
+        <f>aeo_hdd_projections!S3/aeo_hdd_projections!$J3</f>
+        <v>0.91473471292982733</v>
+      </c>
+      <c r="L3" s="13">
+        <f>aeo_hdd_projections!T3/aeo_hdd_projections!$J3</f>
+        <v>0.91240080908666565</v>
+      </c>
+      <c r="M3" s="13">
+        <f>aeo_hdd_projections!U3/aeo_hdd_projections!$J3</f>
+        <v>0.91006690524350398</v>
+      </c>
+      <c r="N3" s="13">
+        <f>aeo_hdd_projections!V3/aeo_hdd_projections!$J3</f>
+        <v>0.9077330014003423</v>
+      </c>
+      <c r="O3" s="13">
+        <f>aeo_hdd_projections!W3/aeo_hdd_projections!$J3</f>
+        <v>0.90539909755718062</v>
+      </c>
+      <c r="P3" s="13">
+        <f>aeo_hdd_projections!X3/aeo_hdd_projections!$J3</f>
+        <v>0.90306519371401894</v>
+      </c>
+      <c r="Q3" s="13">
+        <f>aeo_hdd_projections!Y3/aeo_hdd_projections!$J3</f>
+        <v>0.90088688346040147</v>
+      </c>
+      <c r="R3" s="13">
+        <f>aeo_hdd_projections!Z3/aeo_hdd_projections!$J3</f>
+        <v>0.89855297961723979</v>
+      </c>
+      <c r="S3" s="13">
+        <f>aeo_hdd_projections!AA3/aeo_hdd_projections!$J3</f>
+        <v>0.89621907577407811</v>
+      </c>
+      <c r="T3" s="13">
+        <f>aeo_hdd_projections!AB3/aeo_hdd_projections!$J3</f>
+        <v>0.89388517193091643</v>
+      </c>
+      <c r="U3" s="13">
+        <f>aeo_hdd_projections!AC3/aeo_hdd_projections!$J3</f>
+        <v>0.89155126808775476</v>
+      </c>
+      <c r="V3" s="13">
+        <f>aeo_hdd_projections!AD3/aeo_hdd_projections!$J3</f>
+        <v>0.88921736424459308</v>
+      </c>
+      <c r="W3" s="13">
+        <f>aeo_hdd_projections!AE3/aeo_hdd_projections!$J3</f>
+        <v>0.8870390539909756</v>
+      </c>
+      <c r="X3" s="13">
+        <f>aeo_hdd_projections!AF3/aeo_hdd_projections!$J3</f>
+        <v>0.88470515014781392</v>
+      </c>
+      <c r="Y3" s="13">
+        <f>aeo_hdd_projections!AG3/aeo_hdd_projections!$J3</f>
+        <v>0.88237124630465225</v>
+      </c>
+      <c r="Z3" s="13">
+        <f>aeo_hdd_projections!AH3/aeo_hdd_projections!$J3</f>
+        <v>0.88003734246149057</v>
+      </c>
+      <c r="AA3" s="13">
+        <f>aeo_hdd_projections!AI3/aeo_hdd_projections!$J3</f>
+        <v>0.87770343861832889</v>
+      </c>
+      <c r="AB3" s="13">
+        <f>aeo_hdd_projections!AJ3/aeo_hdd_projections!$J3</f>
+        <v>0.87536953477516721</v>
+      </c>
+      <c r="AC3" s="13">
+        <f>aeo_hdd_projections!AK3/aeo_hdd_projections!$J3</f>
+        <v>0.87303563093200565</v>
+      </c>
+      <c r="AD3" s="13">
+        <f>aeo_hdd_projections!AL3/aeo_hdd_projections!$J3</f>
+        <v>0.87085732067838806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="13">
+        <f>aeo_hdd_projections!$J4/aeo_hdd_projections!$J4</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="13">
+        <f>aeo_hdd_projections!K4/aeo_hdd_projections!$J4</f>
+        <v>0.98709492400344134</v>
+      </c>
+      <c r="D4" s="13">
+        <f>aeo_hdd_projections!L4/aeo_hdd_projections!$J4</f>
+        <v>0.91195870375681098</v>
+      </c>
+      <c r="E4" s="13">
+        <f>aeo_hdd_projections!M4/aeo_hdd_projections!$J4</f>
+        <v>0.90851735015772872</v>
+      </c>
+      <c r="F4" s="13">
+        <f>aeo_hdd_projections!N4/aeo_hdd_projections!$J4</f>
+        <v>0.90507599655864646</v>
+      </c>
+      <c r="G4" s="13">
+        <f>aeo_hdd_projections!O4/aeo_hdd_projections!$J4</f>
+        <v>0.90163464295956408</v>
+      </c>
+      <c r="H4" s="13">
+        <f>aeo_hdd_projections!P4/aeo_hdd_projections!$J4</f>
+        <v>0.89790650989389165</v>
+      </c>
+      <c r="I4" s="13">
+        <f>aeo_hdd_projections!Q4/aeo_hdd_projections!$J4</f>
+        <v>0.89446515629480927</v>
+      </c>
+      <c r="J4" s="13">
+        <f>aeo_hdd_projections!R4/aeo_hdd_projections!$J4</f>
+        <v>0.89073702322913684</v>
+      </c>
+      <c r="K4" s="13">
+        <f>aeo_hdd_projections!S4/aeo_hdd_projections!$J4</f>
+        <v>0.88729566963005446</v>
+      </c>
+      <c r="L4" s="13">
+        <f>aeo_hdd_projections!T4/aeo_hdd_projections!$J4</f>
+        <v>0.88356753656438203</v>
+      </c>
+      <c r="M4" s="13">
+        <f>aeo_hdd_projections!U4/aeo_hdd_projections!$J4</f>
+        <v>0.88012618296529965</v>
+      </c>
+      <c r="N4" s="13">
+        <f>aeo_hdd_projections!V4/aeo_hdd_projections!$J4</f>
+        <v>0.87639804989962722</v>
+      </c>
+      <c r="O4" s="13">
+        <f>aeo_hdd_projections!W4/aeo_hdd_projections!$J4</f>
+        <v>0.87266991683395467</v>
+      </c>
+      <c r="P4" s="13">
+        <f>aeo_hdd_projections!X4/aeo_hdd_projections!$J4</f>
+        <v>0.86922856323487241</v>
+      </c>
+      <c r="Q4" s="13">
+        <f>aeo_hdd_projections!Y4/aeo_hdd_projections!$J4</f>
+        <v>0.86550043016919986</v>
+      </c>
+      <c r="R4" s="13">
+        <f>aeo_hdd_projections!Z4/aeo_hdd_projections!$J4</f>
+        <v>0.86177229710352743</v>
+      </c>
+      <c r="S4" s="13">
+        <f>aeo_hdd_projections!AA4/aeo_hdd_projections!$J4</f>
+        <v>0.85804416403785488</v>
+      </c>
+      <c r="T4" s="13">
+        <f>aeo_hdd_projections!AB4/aeo_hdd_projections!$J4</f>
+        <v>0.85460281043877262</v>
+      </c>
+      <c r="U4" s="13">
+        <f>aeo_hdd_projections!AC4/aeo_hdd_projections!$J4</f>
+        <v>0.85087467737310007</v>
+      </c>
+      <c r="V4" s="13">
+        <f>aeo_hdd_projections!AD4/aeo_hdd_projections!$J4</f>
+        <v>0.84714654430742764</v>
+      </c>
+      <c r="W4" s="13">
+        <f>aeo_hdd_projections!AE4/aeo_hdd_projections!$J4</f>
+        <v>0.84341841124175509</v>
+      </c>
+      <c r="X4" s="13">
+        <f>aeo_hdd_projections!AF4/aeo_hdd_projections!$J4</f>
+        <v>0.83997705764267283</v>
+      </c>
+      <c r="Y4" s="13">
+        <f>aeo_hdd_projections!AG4/aeo_hdd_projections!$J4</f>
+        <v>0.83624892457700029</v>
+      </c>
+      <c r="Z4" s="13">
+        <f>aeo_hdd_projections!AH4/aeo_hdd_projections!$J4</f>
+        <v>0.83252079151132774</v>
+      </c>
+      <c r="AA4" s="13">
+        <f>aeo_hdd_projections!AI4/aeo_hdd_projections!$J4</f>
+        <v>0.82879265844565531</v>
+      </c>
+      <c r="AB4" s="13">
+        <f>aeo_hdd_projections!AJ4/aeo_hdd_projections!$J4</f>
+        <v>0.82506452537998276</v>
+      </c>
+      <c r="AC4" s="13">
+        <f>aeo_hdd_projections!AK4/aeo_hdd_projections!$J4</f>
+        <v>0.8216231717809005</v>
+      </c>
+      <c r="AD4" s="13">
+        <f>aeo_hdd_projections!AL4/aeo_hdd_projections!$J4</f>
+        <v>0.81789503871522795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="13">
+        <f>aeo_hdd_projections!$J5/aeo_hdd_projections!$J5</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="13">
+        <f>aeo_hdd_projections!K5/aeo_hdd_projections!$J5</f>
+        <v>1.0064437478230581</v>
+      </c>
+      <c r="D5" s="13">
+        <f>aeo_hdd_projections!L5/aeo_hdd_projections!$J5</f>
+        <v>0.93138279345175901</v>
+      </c>
+      <c r="E5" s="13">
+        <f>aeo_hdd_projections!M5/aeo_hdd_projections!$J5</f>
+        <v>0.92737722048066873</v>
+      </c>
+      <c r="F5" s="13">
+        <f>aeo_hdd_projections!N5/aeo_hdd_projections!$J5</f>
+        <v>0.92354580285614774</v>
+      </c>
+      <c r="G5" s="13">
+        <f>aeo_hdd_projections!O5/aeo_hdd_projections!$J5</f>
+        <v>0.91971438523162663</v>
+      </c>
+      <c r="H5" s="13">
+        <f>aeo_hdd_projections!P5/aeo_hdd_projections!$J5</f>
+        <v>0.91588296760710552</v>
+      </c>
+      <c r="I5" s="13">
+        <f>aeo_hdd_projections!Q5/aeo_hdd_projections!$J5</f>
+        <v>0.91187739463601536</v>
+      </c>
+      <c r="J5" s="13">
+        <f>aeo_hdd_projections!R5/aeo_hdd_projections!$J5</f>
+        <v>0.90804597701149425</v>
+      </c>
+      <c r="K5" s="13">
+        <f>aeo_hdd_projections!S5/aeo_hdd_projections!$J5</f>
+        <v>0.90421455938697315</v>
+      </c>
+      <c r="L5" s="13">
+        <f>aeo_hdd_projections!T5/aeo_hdd_projections!$J5</f>
+        <v>0.90020898641588298</v>
+      </c>
+      <c r="M5" s="13">
+        <f>aeo_hdd_projections!U5/aeo_hdd_projections!$J5</f>
+        <v>0.89637756879136188</v>
+      </c>
+      <c r="N5" s="13">
+        <f>aeo_hdd_projections!V5/aeo_hdd_projections!$J5</f>
+        <v>0.89254615116684077</v>
+      </c>
+      <c r="O5" s="13">
+        <f>aeo_hdd_projections!W5/aeo_hdd_projections!$J5</f>
+        <v>0.88854057819575061</v>
+      </c>
+      <c r="P5" s="13">
+        <f>aeo_hdd_projections!X5/aeo_hdd_projections!$J5</f>
+        <v>0.8847091605712295</v>
+      </c>
+      <c r="Q5" s="13">
+        <f>aeo_hdd_projections!Y5/aeo_hdd_projections!$J5</f>
+        <v>0.88087774294670851</v>
+      </c>
+      <c r="R5" s="13">
+        <f>aeo_hdd_projections!Z5/aeo_hdd_projections!$J5</f>
+        <v>0.8770463253221874</v>
+      </c>
+      <c r="S5" s="13">
+        <f>aeo_hdd_projections!AA5/aeo_hdd_projections!$J5</f>
+        <v>0.87304075235109713</v>
+      </c>
+      <c r="T5" s="13">
+        <f>aeo_hdd_projections!AB5/aeo_hdd_projections!$J5</f>
+        <v>0.86920933472657613</v>
+      </c>
+      <c r="U5" s="13">
+        <f>aeo_hdd_projections!AC5/aeo_hdd_projections!$J5</f>
+        <v>0.86537791710205503</v>
+      </c>
+      <c r="V5" s="13">
+        <f>aeo_hdd_projections!AD5/aeo_hdd_projections!$J5</f>
+        <v>0.86154649947753392</v>
+      </c>
+      <c r="W5" s="13">
+        <f>aeo_hdd_projections!AE5/aeo_hdd_projections!$J5</f>
+        <v>0.85754092650644376</v>
+      </c>
+      <c r="X5" s="13">
+        <f>aeo_hdd_projections!AF5/aeo_hdd_projections!$J5</f>
+        <v>0.85370950888192265</v>
+      </c>
+      <c r="Y5" s="13">
+        <f>aeo_hdd_projections!AG5/aeo_hdd_projections!$J5</f>
+        <v>0.84987809125740155</v>
+      </c>
+      <c r="Z5" s="13">
+        <f>aeo_hdd_projections!AH5/aeo_hdd_projections!$J5</f>
+        <v>0.84604667363288055</v>
+      </c>
+      <c r="AA5" s="13">
+        <f>aeo_hdd_projections!AI5/aeo_hdd_projections!$J5</f>
+        <v>0.84204110066179028</v>
+      </c>
+      <c r="AB5" s="13">
+        <f>aeo_hdd_projections!AJ5/aeo_hdd_projections!$J5</f>
+        <v>0.83820968303726928</v>
+      </c>
+      <c r="AC5" s="13">
+        <f>aeo_hdd_projections!AK5/aeo_hdd_projections!$J5</f>
+        <v>0.83437826541274818</v>
+      </c>
+      <c r="AD5" s="13">
+        <f>aeo_hdd_projections!AL5/aeo_hdd_projections!$J5</f>
+        <v>0.83054684778822707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" s="13">
+        <f>aeo_hdd_projections!$J6/aeo_hdd_projections!$J6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="13">
+        <f>aeo_hdd_projections!K6/aeo_hdd_projections!$J6</f>
+        <v>1.0016096579476861</v>
+      </c>
+      <c r="D6" s="13">
+        <f>aeo_hdd_projections!L6/aeo_hdd_projections!$J6</f>
+        <v>0.96358148893360163</v>
+      </c>
+      <c r="E6" s="13">
+        <f>aeo_hdd_projections!M6/aeo_hdd_projections!$J6</f>
+        <v>0.96096579476861166</v>
+      </c>
+      <c r="F6" s="13">
+        <f>aeo_hdd_projections!N6/aeo_hdd_projections!$J6</f>
+        <v>0.95835010060362169</v>
+      </c>
+      <c r="G6" s="13">
+        <f>aeo_hdd_projections!O6/aeo_hdd_projections!$J6</f>
+        <v>0.95593561368209257</v>
+      </c>
+      <c r="H6" s="13">
+        <f>aeo_hdd_projections!P6/aeo_hdd_projections!$J6</f>
+        <v>0.9533199195171026</v>
+      </c>
+      <c r="I6" s="13">
+        <f>aeo_hdd_projections!Q6/aeo_hdd_projections!$J6</f>
+        <v>0.95070422535211263</v>
+      </c>
+      <c r="J6" s="13">
+        <f>aeo_hdd_projections!R6/aeo_hdd_projections!$J6</f>
+        <v>0.94808853118712277</v>
+      </c>
+      <c r="K6" s="13">
+        <f>aeo_hdd_projections!S6/aeo_hdd_projections!$J6</f>
+        <v>0.94527162977867207</v>
+      </c>
+      <c r="L6" s="13">
+        <f>aeo_hdd_projections!T6/aeo_hdd_projections!$J6</f>
+        <v>0.94265593561368211</v>
+      </c>
+      <c r="M6" s="13">
+        <f>aeo_hdd_projections!U6/aeo_hdd_projections!$J6</f>
+        <v>0.94004024144869214</v>
+      </c>
+      <c r="N6" s="13">
+        <f>aeo_hdd_projections!V6/aeo_hdd_projections!$J6</f>
+        <v>0.93722334004024144</v>
+      </c>
+      <c r="O6" s="13">
+        <f>aeo_hdd_projections!W6/aeo_hdd_projections!$J6</f>
+        <v>0.93460764587525147</v>
+      </c>
+      <c r="P6" s="13">
+        <f>aeo_hdd_projections!X6/aeo_hdd_projections!$J6</f>
+        <v>0.93199195171026161</v>
+      </c>
+      <c r="Q6" s="13">
+        <f>aeo_hdd_projections!Y6/aeo_hdd_projections!$J6</f>
+        <v>0.92937625754527164</v>
+      </c>
+      <c r="R6" s="13">
+        <f>aeo_hdd_projections!Z6/aeo_hdd_projections!$J6</f>
+        <v>0.92676056338028168</v>
+      </c>
+      <c r="S6" s="13">
+        <f>aeo_hdd_projections!AA6/aeo_hdd_projections!$J6</f>
+        <v>0.92414486921529171</v>
+      </c>
+      <c r="T6" s="13">
+        <f>aeo_hdd_projections!AB6/aeo_hdd_projections!$J6</f>
+        <v>0.92152917505030185</v>
+      </c>
+      <c r="U6" s="13">
+        <f>aeo_hdd_projections!AC6/aeo_hdd_projections!$J6</f>
+        <v>0.91911468812877262</v>
+      </c>
+      <c r="V6" s="13">
+        <f>aeo_hdd_projections!AD6/aeo_hdd_projections!$J6</f>
+        <v>0.91649899396378265</v>
+      </c>
+      <c r="W6" s="13">
+        <f>aeo_hdd_projections!AE6/aeo_hdd_projections!$J6</f>
+        <v>0.91388329979879279</v>
+      </c>
+      <c r="X6" s="13">
+        <f>aeo_hdd_projections!AF6/aeo_hdd_projections!$J6</f>
+        <v>0.91146881287726356</v>
+      </c>
+      <c r="Y6" s="13">
+        <f>aeo_hdd_projections!AG6/aeo_hdd_projections!$J6</f>
+        <v>0.90885311871227359</v>
+      </c>
+      <c r="Z6" s="13">
+        <f>aeo_hdd_projections!AH6/aeo_hdd_projections!$J6</f>
+        <v>0.90623742454728373</v>
+      </c>
+      <c r="AA6" s="13">
+        <f>aeo_hdd_projections!AI6/aeo_hdd_projections!$J6</f>
+        <v>0.9038229376257545</v>
+      </c>
+      <c r="AB6" s="13">
+        <f>aeo_hdd_projections!AJ6/aeo_hdd_projections!$J6</f>
+        <v>0.90120724346076464</v>
+      </c>
+      <c r="AC6" s="13">
+        <f>aeo_hdd_projections!AK6/aeo_hdd_projections!$J6</f>
+        <v>0.8987927565392354</v>
+      </c>
+      <c r="AD6" s="13">
+        <f>aeo_hdd_projections!AL6/aeo_hdd_projections!$J6</f>
+        <v>0.89617706237424544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="13">
+        <f>aeo_hdd_projections!$J7/aeo_hdd_projections!$J7</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="13">
+        <f>aeo_hdd_projections!K7/aeo_hdd_projections!$J7</f>
+        <v>1.0358180058083253</v>
+      </c>
+      <c r="D7" s="13">
+        <f>aeo_hdd_projections!L7/aeo_hdd_projections!$J7</f>
+        <v>0.96353662471765089</v>
+      </c>
+      <c r="E7" s="13">
+        <f>aeo_hdd_projections!M7/aeo_hdd_projections!$J7</f>
+        <v>0.95982575024201355</v>
+      </c>
+      <c r="F7" s="13">
+        <f>aeo_hdd_projections!N7/aeo_hdd_projections!$J7</f>
+        <v>0.95595353339787026</v>
+      </c>
+      <c r="G7" s="13">
+        <f>aeo_hdd_projections!O7/aeo_hdd_projections!$J7</f>
+        <v>0.95224265892223303</v>
+      </c>
+      <c r="H7" s="13">
+        <f>aeo_hdd_projections!P7/aeo_hdd_projections!$J7</f>
+        <v>0.94837044207808974</v>
+      </c>
+      <c r="I7" s="13">
+        <f>aeo_hdd_projections!Q7/aeo_hdd_projections!$J7</f>
+        <v>0.94449822523394644</v>
+      </c>
+      <c r="J7" s="13">
+        <f>aeo_hdd_projections!R7/aeo_hdd_projections!$J7</f>
+        <v>0.94062600838980315</v>
+      </c>
+      <c r="K7" s="13">
+        <f>aeo_hdd_projections!S7/aeo_hdd_projections!$J7</f>
+        <v>0.93691513391416581</v>
+      </c>
+      <c r="L7" s="13">
+        <f>aeo_hdd_projections!T7/aeo_hdd_projections!$J7</f>
+        <v>0.93304291707002263</v>
+      </c>
+      <c r="M7" s="13">
+        <f>aeo_hdd_projections!U7/aeo_hdd_projections!$J7</f>
+        <v>0.92917070022587933</v>
+      </c>
+      <c r="N7" s="13">
+        <f>aeo_hdd_projections!V7/aeo_hdd_projections!$J7</f>
+        <v>0.92529848338173604</v>
+      </c>
+      <c r="O7" s="13">
+        <f>aeo_hdd_projections!W7/aeo_hdd_projections!$J7</f>
+        <v>0.92142626653759274</v>
+      </c>
+      <c r="P7" s="13">
+        <f>aeo_hdd_projections!X7/aeo_hdd_projections!$J7</f>
+        <v>0.91755404969344945</v>
+      </c>
+      <c r="Q7" s="13">
+        <f>aeo_hdd_projections!Y7/aeo_hdd_projections!$J7</f>
+        <v>0.91368183284930626</v>
+      </c>
+      <c r="R7" s="13">
+        <f>aeo_hdd_projections!Z7/aeo_hdd_projections!$J7</f>
+        <v>0.90980961600516297</v>
+      </c>
+      <c r="S7" s="13">
+        <f>aeo_hdd_projections!AA7/aeo_hdd_projections!$J7</f>
+        <v>0.90593739916101967</v>
+      </c>
+      <c r="T7" s="13">
+        <f>aeo_hdd_projections!AB7/aeo_hdd_projections!$J7</f>
+        <v>0.90206518231687638</v>
+      </c>
+      <c r="U7" s="13">
+        <f>aeo_hdd_projections!AC7/aeo_hdd_projections!$J7</f>
+        <v>0.89819296547273308</v>
+      </c>
+      <c r="V7" s="13">
+        <f>aeo_hdd_projections!AD7/aeo_hdd_projections!$J7</f>
+        <v>0.8943207486285899</v>
+      </c>
+      <c r="W7" s="13">
+        <f>aeo_hdd_projections!AE7/aeo_hdd_projections!$J7</f>
+        <v>0.89044853178444661</v>
+      </c>
+      <c r="X7" s="13">
+        <f>aeo_hdd_projections!AF7/aeo_hdd_projections!$J7</f>
+        <v>0.88657631494030331</v>
+      </c>
+      <c r="Y7" s="13">
+        <f>aeo_hdd_projections!AG7/aeo_hdd_projections!$J7</f>
+        <v>0.88270409809616002</v>
+      </c>
+      <c r="Z7" s="13">
+        <f>aeo_hdd_projections!AH7/aeo_hdd_projections!$J7</f>
+        <v>0.87883188125201683</v>
+      </c>
+      <c r="AA7" s="13">
+        <f>aeo_hdd_projections!AI7/aeo_hdd_projections!$J7</f>
+        <v>0.87495966440787354</v>
+      </c>
+      <c r="AB7" s="13">
+        <f>aeo_hdd_projections!AJ7/aeo_hdd_projections!$J7</f>
+        <v>0.87108744756373024</v>
+      </c>
+      <c r="AC7" s="13">
+        <f>aeo_hdd_projections!AK7/aeo_hdd_projections!$J7</f>
+        <v>0.86705388835108099</v>
+      </c>
+      <c r="AD7" s="13">
+        <f>aeo_hdd_projections!AL7/aeo_hdd_projections!$J7</f>
+        <v>0.8631816715069377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="13">
+        <f>aeo_hdd_projections!$J8/aeo_hdd_projections!$J8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="13">
+        <f>aeo_hdd_projections!K8/aeo_hdd_projections!$J8</f>
+        <v>1.0905977584059776</v>
+      </c>
+      <c r="D8" s="13">
+        <f>aeo_hdd_projections!L8/aeo_hdd_projections!$J8</f>
+        <v>1.0118306351183064</v>
+      </c>
+      <c r="E8" s="13">
+        <f>aeo_hdd_projections!M8/aeo_hdd_projections!$J8</f>
+        <v>1.0090286425902864</v>
+      </c>
+      <c r="F8" s="13">
+        <f>aeo_hdd_projections!N8/aeo_hdd_projections!$J8</f>
+        <v>1.0062266500622665</v>
+      </c>
+      <c r="G8" s="13">
+        <f>aeo_hdd_projections!O8/aeo_hdd_projections!$J8</f>
+        <v>1.0034246575342465</v>
+      </c>
+      <c r="H8" s="13">
+        <f>aeo_hdd_projections!P8/aeo_hdd_projections!$J8</f>
+        <v>1.0003113325031132</v>
+      </c>
+      <c r="I8" s="13">
+        <f>aeo_hdd_projections!Q8/aeo_hdd_projections!$J8</f>
+        <v>0.99750933997509339</v>
+      </c>
+      <c r="J8" s="13">
+        <f>aeo_hdd_projections!R8/aeo_hdd_projections!$J8</f>
+        <v>0.99470734744707345</v>
+      </c>
+      <c r="K8" s="13">
+        <f>aeo_hdd_projections!S8/aeo_hdd_projections!$J8</f>
+        <v>0.99159402241594019</v>
+      </c>
+      <c r="L8" s="13">
+        <f>aeo_hdd_projections!T8/aeo_hdd_projections!$J8</f>
+        <v>0.98879202988792025</v>
+      </c>
+      <c r="M8" s="13">
+        <f>aeo_hdd_projections!U8/aeo_hdd_projections!$J8</f>
+        <v>0.9856787048567871</v>
+      </c>
+      <c r="N8" s="13">
+        <f>aeo_hdd_projections!V8/aeo_hdd_projections!$J8</f>
+        <v>0.98287671232876717</v>
+      </c>
+      <c r="O8" s="13">
+        <f>aeo_hdd_projections!W8/aeo_hdd_projections!$J8</f>
+        <v>0.9797633872976339</v>
+      </c>
+      <c r="P8" s="13">
+        <f>aeo_hdd_projections!X8/aeo_hdd_projections!$J8</f>
+        <v>0.97665006226650064</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>aeo_hdd_projections!Y8/aeo_hdd_projections!$J8</f>
+        <v>0.9738480697384807</v>
+      </c>
+      <c r="R8" s="13">
+        <f>aeo_hdd_projections!Z8/aeo_hdd_projections!$J8</f>
+        <v>0.97073474470734744</v>
+      </c>
+      <c r="S8" s="13">
+        <f>aeo_hdd_projections!AA8/aeo_hdd_projections!$J8</f>
+        <v>0.96762141967621418</v>
+      </c>
+      <c r="T8" s="13">
+        <f>aeo_hdd_projections!AB8/aeo_hdd_projections!$J8</f>
+        <v>0.96450809464508092</v>
+      </c>
+      <c r="U8" s="13">
+        <f>aeo_hdd_projections!AC8/aeo_hdd_projections!$J8</f>
+        <v>0.96170610211706098</v>
+      </c>
+      <c r="V8" s="13">
+        <f>aeo_hdd_projections!AD8/aeo_hdd_projections!$J8</f>
+        <v>0.95859277708592772</v>
+      </c>
+      <c r="W8" s="13">
+        <f>aeo_hdd_projections!AE8/aeo_hdd_projections!$J8</f>
+        <v>0.95547945205479456</v>
+      </c>
+      <c r="X8" s="13">
+        <f>aeo_hdd_projections!AF8/aeo_hdd_projections!$J8</f>
+        <v>0.9523661270236613</v>
+      </c>
+      <c r="Y8" s="13">
+        <f>aeo_hdd_projections!AG8/aeo_hdd_projections!$J8</f>
+        <v>0.94925280199252804</v>
+      </c>
+      <c r="Z8" s="13">
+        <f>aeo_hdd_projections!AH8/aeo_hdd_projections!$J8</f>
+        <v>0.9464508094645081</v>
+      </c>
+      <c r="AA8" s="13">
+        <f>aeo_hdd_projections!AI8/aeo_hdd_projections!$J8</f>
+        <v>0.94333748443337484</v>
+      </c>
+      <c r="AB8" s="13">
+        <f>aeo_hdd_projections!AJ8/aeo_hdd_projections!$J8</f>
+        <v>0.94022415940224158</v>
+      </c>
+      <c r="AC8" s="13">
+        <f>aeo_hdd_projections!AK8/aeo_hdd_projections!$J8</f>
+        <v>0.93711083437110831</v>
+      </c>
+      <c r="AD8" s="13">
+        <f>aeo_hdd_projections!AL8/aeo_hdd_projections!$J8</f>
+        <v>0.93399750933997505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="13">
+        <f>aeo_hdd_projections!$J9/aeo_hdd_projections!$J9</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="13">
+        <f>aeo_hdd_projections!K9/aeo_hdd_projections!$J9</f>
+        <v>1.0132501948558068</v>
+      </c>
+      <c r="D9" s="13">
+        <f>aeo_hdd_projections!L9/aeo_hdd_projections!$J9</f>
+        <v>0.92556508183943886</v>
+      </c>
+      <c r="E9" s="13">
+        <f>aeo_hdd_projections!M9/aeo_hdd_projections!$J9</f>
+        <v>0.91893998441153546</v>
+      </c>
+      <c r="F9" s="13">
+        <f>aeo_hdd_projections!N9/aeo_hdd_projections!$J9</f>
+        <v>0.91270459859703823</v>
+      </c>
+      <c r="G9" s="13">
+        <f>aeo_hdd_projections!O9/aeo_hdd_projections!$J9</f>
+        <v>0.90646921278254089</v>
+      </c>
+      <c r="H9" s="13">
+        <f>aeo_hdd_projections!P9/aeo_hdd_projections!$J9</f>
+        <v>0.90023382696804366</v>
+      </c>
+      <c r="I9" s="13">
+        <f>aeo_hdd_projections!Q9/aeo_hdd_projections!$J9</f>
+        <v>0.89399844115354643</v>
+      </c>
+      <c r="J9" s="13">
+        <f>aeo_hdd_projections!R9/aeo_hdd_projections!$J9</f>
+        <v>0.88737334372564303</v>
+      </c>
+      <c r="K9" s="13">
+        <f>aeo_hdd_projections!S9/aeo_hdd_projections!$J9</f>
+        <v>0.8811379579111458</v>
+      </c>
+      <c r="L9" s="13">
+        <f>aeo_hdd_projections!T9/aeo_hdd_projections!$J9</f>
+        <v>0.87490257209664846</v>
+      </c>
+      <c r="M9" s="13">
+        <f>aeo_hdd_projections!U9/aeo_hdd_projections!$J9</f>
+        <v>0.86866718628215123</v>
+      </c>
+      <c r="N9" s="13">
+        <f>aeo_hdd_projections!V9/aeo_hdd_projections!$J9</f>
+        <v>0.86243180046765389</v>
+      </c>
+      <c r="O9" s="13">
+        <f>aeo_hdd_projections!W9/aeo_hdd_projections!$J9</f>
+        <v>0.85619641465315666</v>
+      </c>
+      <c r="P9" s="13">
+        <f>aeo_hdd_projections!X9/aeo_hdd_projections!$J9</f>
+        <v>0.84957131722525336</v>
+      </c>
+      <c r="Q9" s="13">
+        <f>aeo_hdd_projections!Y9/aeo_hdd_projections!$J9</f>
+        <v>0.84333593141075602</v>
+      </c>
+      <c r="R9" s="13">
+        <f>aeo_hdd_projections!Z9/aeo_hdd_projections!$J9</f>
+        <v>0.83710054559625879</v>
+      </c>
+      <c r="S9" s="13">
+        <f>aeo_hdd_projections!AA9/aeo_hdd_projections!$J9</f>
+        <v>0.83086515978176145</v>
+      </c>
+      <c r="T9" s="13">
+        <f>aeo_hdd_projections!AB9/aeo_hdd_projections!$J9</f>
+        <v>0.82462977396726422</v>
+      </c>
+      <c r="U9" s="13">
+        <f>aeo_hdd_projections!AC9/aeo_hdd_projections!$J9</f>
+        <v>0.81839438815276699</v>
+      </c>
+      <c r="V9" s="13">
+        <f>aeo_hdd_projections!AD9/aeo_hdd_projections!$J9</f>
+        <v>0.81215900233826965</v>
+      </c>
+      <c r="W9" s="13">
+        <f>aeo_hdd_projections!AE9/aeo_hdd_projections!$J9</f>
+        <v>0.80592361652377242</v>
+      </c>
+      <c r="X9" s="13">
+        <f>aeo_hdd_projections!AF9/aeo_hdd_projections!$J9</f>
+        <v>0.79968823070927508</v>
+      </c>
+      <c r="Y9" s="13">
+        <f>aeo_hdd_projections!AG9/aeo_hdd_projections!$J9</f>
+        <v>0.79345284489477785</v>
+      </c>
+      <c r="Z9" s="13">
+        <f>aeo_hdd_projections!AH9/aeo_hdd_projections!$J9</f>
+        <v>0.78721745908028062</v>
+      </c>
+      <c r="AA9" s="13">
+        <f>aeo_hdd_projections!AI9/aeo_hdd_projections!$J9</f>
+        <v>0.78137178487918935</v>
+      </c>
+      <c r="AB9" s="13">
+        <f>aeo_hdd_projections!AJ9/aeo_hdd_projections!$J9</f>
+        <v>0.77513639906469212</v>
+      </c>
+      <c r="AC9" s="13">
+        <f>aeo_hdd_projections!AK9/aeo_hdd_projections!$J9</f>
+        <v>0.76890101325019489</v>
+      </c>
+      <c r="AD9" s="13">
+        <f>aeo_hdd_projections!AL9/aeo_hdd_projections!$J9</f>
+        <v>0.76266562743569755</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="13">
+        <f>aeo_hdd_projections!$J10/aeo_hdd_projections!$J10</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <f>aeo_hdd_projections!K10/aeo_hdd_projections!$J10</f>
+        <v>0.96435354273192109</v>
+      </c>
+      <c r="D10" s="13">
+        <f>aeo_hdd_projections!L10/aeo_hdd_projections!$J10</f>
+        <v>0.9275383491599708</v>
+      </c>
+      <c r="E10" s="13">
+        <f>aeo_hdd_projections!M10/aeo_hdd_projections!$J10</f>
+        <v>0.92622352081811543</v>
+      </c>
+      <c r="F10" s="13">
+        <f>aeo_hdd_projections!N10/aeo_hdd_projections!$J10</f>
+        <v>0.92476260043827607</v>
+      </c>
+      <c r="G10" s="13">
+        <f>aeo_hdd_projections!O10/aeo_hdd_projections!$J10</f>
+        <v>0.9234477720964207</v>
+      </c>
+      <c r="H10" s="13">
+        <f>aeo_hdd_projections!P10/aeo_hdd_projections!$J10</f>
+        <v>0.92198685171658146</v>
+      </c>
+      <c r="I10" s="13">
+        <f>aeo_hdd_projections!Q10/aeo_hdd_projections!$J10</f>
+        <v>0.9205259313367421</v>
+      </c>
+      <c r="J10" s="13">
+        <f>aeo_hdd_projections!R10/aeo_hdd_projections!$J10</f>
+        <v>0.91906501095690285</v>
+      </c>
+      <c r="K10" s="13">
+        <f>aeo_hdd_projections!S10/aeo_hdd_projections!$J10</f>
+        <v>0.9176040905770636</v>
+      </c>
+      <c r="L10" s="13">
+        <f>aeo_hdd_projections!T10/aeo_hdd_projections!$J10</f>
+        <v>0.91614317019722424</v>
+      </c>
+      <c r="M10" s="13">
+        <f>aeo_hdd_projections!U10/aeo_hdd_projections!$J10</f>
+        <v>0.914682249817385</v>
+      </c>
+      <c r="N10" s="13">
+        <f>aeo_hdd_projections!V10/aeo_hdd_projections!$J10</f>
+        <v>0.91307523739956176</v>
+      </c>
+      <c r="O10" s="13">
+        <f>aeo_hdd_projections!W10/aeo_hdd_projections!$J10</f>
+        <v>0.9116143170197224</v>
+      </c>
+      <c r="P10" s="13">
+        <f>aeo_hdd_projections!X10/aeo_hdd_projections!$J10</f>
+        <v>0.91015339663988315</v>
+      </c>
+      <c r="Q10" s="13">
+        <f>aeo_hdd_projections!Y10/aeo_hdd_projections!$J10</f>
+        <v>0.90854638422205991</v>
+      </c>
+      <c r="R10" s="13">
+        <f>aeo_hdd_projections!Z10/aeo_hdd_projections!$J10</f>
+        <v>0.90708546384222055</v>
+      </c>
+      <c r="S10" s="13">
+        <f>aeo_hdd_projections!AA10/aeo_hdd_projections!$J10</f>
+        <v>0.90547845142439742</v>
+      </c>
+      <c r="T10" s="13">
+        <f>aeo_hdd_projections!AB10/aeo_hdd_projections!$J10</f>
+        <v>0.90401753104455806</v>
+      </c>
+      <c r="U10" s="13">
+        <f>aeo_hdd_projections!AC10/aeo_hdd_projections!$J10</f>
+        <v>0.90241051862673483</v>
+      </c>
+      <c r="V10" s="13">
+        <f>aeo_hdd_projections!AD10/aeo_hdd_projections!$J10</f>
+        <v>0.90094959824689558</v>
+      </c>
+      <c r="W10" s="13">
+        <f>aeo_hdd_projections!AE10/aeo_hdd_projections!$J10</f>
+        <v>0.89934258582907234</v>
+      </c>
+      <c r="X10" s="13">
+        <f>aeo_hdd_projections!AF10/aeo_hdd_projections!$J10</f>
+        <v>0.8977355734112491</v>
+      </c>
+      <c r="Y10" s="13">
+        <f>aeo_hdd_projections!AG10/aeo_hdd_projections!$J10</f>
+        <v>0.89627465303140974</v>
+      </c>
+      <c r="Z10" s="13">
+        <f>aeo_hdd_projections!AH10/aeo_hdd_projections!$J10</f>
+        <v>0.89466764061358661</v>
+      </c>
+      <c r="AA10" s="13">
+        <f>aeo_hdd_projections!AI10/aeo_hdd_projections!$J10</f>
+        <v>0.89306062819576337</v>
+      </c>
+      <c r="AB10" s="13">
+        <f>aeo_hdd_projections!AJ10/aeo_hdd_projections!$J10</f>
+        <v>0.89159970781592401</v>
+      </c>
+      <c r="AC10" s="13">
+        <f>aeo_hdd_projections!AK10/aeo_hdd_projections!$J10</f>
+        <v>0.88999269539810077</v>
+      </c>
+      <c r="AD10" s="13">
+        <f>aeo_hdd_projections!AL10/aeo_hdd_projections!$J10</f>
+        <v>0.88838568298027754</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="13">
+        <f>aeo_hdd_projections!$J11/aeo_hdd_projections!$J11</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <f>aeo_hdd_projections!K11/aeo_hdd_projections!$J11</f>
+        <v>0.93667425968109341</v>
+      </c>
+      <c r="D11" s="13">
+        <f>aeo_hdd_projections!L11/aeo_hdd_projections!$J11</f>
+        <v>0.88473804100227793</v>
+      </c>
+      <c r="E11" s="13">
+        <f>aeo_hdd_projections!M11/aeo_hdd_projections!$J11</f>
+        <v>0.8810933940774488</v>
+      </c>
+      <c r="F11" s="13">
+        <f>aeo_hdd_projections!N11/aeo_hdd_projections!$J11</f>
+        <v>0.87699316628701596</v>
+      </c>
+      <c r="G11" s="13">
+        <f>aeo_hdd_projections!O11/aeo_hdd_projections!$J11</f>
+        <v>0.87289293849658312</v>
+      </c>
+      <c r="H11" s="13">
+        <f>aeo_hdd_projections!P11/aeo_hdd_projections!$J11</f>
+        <v>0.86924829157175398</v>
+      </c>
+      <c r="I11" s="13">
+        <f>aeo_hdd_projections!Q11/aeo_hdd_projections!$J11</f>
+        <v>0.86514806378132114</v>
+      </c>
+      <c r="J11" s="13">
+        <f>aeo_hdd_projections!R11/aeo_hdd_projections!$J11</f>
+        <v>0.86150341685649201</v>
+      </c>
+      <c r="K11" s="13">
+        <f>aeo_hdd_projections!S11/aeo_hdd_projections!$J11</f>
+        <v>0.85740318906605928</v>
+      </c>
+      <c r="L11" s="13">
+        <f>aeo_hdd_projections!T11/aeo_hdd_projections!$J11</f>
+        <v>0.85375854214123004</v>
+      </c>
+      <c r="M11" s="13">
+        <f>aeo_hdd_projections!U11/aeo_hdd_projections!$J11</f>
+        <v>0.84965831435079731</v>
+      </c>
+      <c r="N11" s="13">
+        <f>aeo_hdd_projections!V11/aeo_hdd_projections!$J11</f>
+        <v>0.84601366742596806</v>
+      </c>
+      <c r="O11" s="13">
+        <f>aeo_hdd_projections!W11/aeo_hdd_projections!$J11</f>
+        <v>0.84236902050113893</v>
+      </c>
+      <c r="P11" s="13">
+        <f>aeo_hdd_projections!X11/aeo_hdd_projections!$J11</f>
+        <v>0.8382687927107062</v>
+      </c>
+      <c r="Q11" s="13">
+        <f>aeo_hdd_projections!Y11/aeo_hdd_projections!$J11</f>
+        <v>0.83462414578587696</v>
+      </c>
+      <c r="R11" s="13">
+        <f>aeo_hdd_projections!Z11/aeo_hdd_projections!$J11</f>
+        <v>0.83097949886104783</v>
+      </c>
+      <c r="S11" s="13">
+        <f>aeo_hdd_projections!AA11/aeo_hdd_projections!$J11</f>
+        <v>0.82687927107061499</v>
+      </c>
+      <c r="T11" s="13">
+        <f>aeo_hdd_projections!AB11/aeo_hdd_projections!$J11</f>
+        <v>0.82323462414578585</v>
+      </c>
+      <c r="U11" s="13">
+        <f>aeo_hdd_projections!AC11/aeo_hdd_projections!$J11</f>
+        <v>0.81958997722095672</v>
+      </c>
+      <c r="V11" s="13">
+        <f>aeo_hdd_projections!AD11/aeo_hdd_projections!$J11</f>
+        <v>0.81594533029612759</v>
+      </c>
+      <c r="W11" s="13">
+        <f>aeo_hdd_projections!AE11/aeo_hdd_projections!$J11</f>
+        <v>0.81230068337129846</v>
+      </c>
+      <c r="X11" s="13">
+        <f>aeo_hdd_projections!AF11/aeo_hdd_projections!$J11</f>
+        <v>0.80820045558086562</v>
+      </c>
+      <c r="Y11" s="13">
+        <f>aeo_hdd_projections!AG11/aeo_hdd_projections!$J11</f>
+        <v>0.80455580865603649</v>
+      </c>
+      <c r="Z11" s="13">
+        <f>aeo_hdd_projections!AH11/aeo_hdd_projections!$J11</f>
+        <v>0.80091116173120724</v>
+      </c>
+      <c r="AA11" s="13">
+        <f>aeo_hdd_projections!AI11/aeo_hdd_projections!$J11</f>
+        <v>0.79726651480637811</v>
+      </c>
+      <c r="AB11" s="13">
+        <f>aeo_hdd_projections!AJ11/aeo_hdd_projections!$J11</f>
+        <v>0.79362186788154898</v>
+      </c>
+      <c r="AC11" s="13">
+        <f>aeo_hdd_projections!AK11/aeo_hdd_projections!$J11</f>
+        <v>0.78997722095671985</v>
+      </c>
+      <c r="AD11" s="13">
+        <f>aeo_hdd_projections!AL11/aeo_hdd_projections!$J11</f>
+        <v>0.78633257403189061</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9CC790-CA46-4AEA-B239-800BEEC2BF59}">
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60937,7 +62288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F2A8E9-CD99-41A6-AC11-BBCC1A6899F0}">
   <dimension ref="A1:I118"/>
   <sheetViews>
@@ -61988,7 +63339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AFB96A0-AB91-4B02-B4D8-9B10B4BD9B3D}">
   <dimension ref="A1:G117"/>
   <sheetViews>
@@ -64352,7 +65703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8DE1A6-D66C-48AB-A787-1C6D7AD77924}">
   <dimension ref="A1:G123"/>
   <sheetViews>

</xml_diff>

<commit_message>
refactor code to handle multipe scenarios without crashing
</commit_message>
<xml_diff>
--- a/projections/aeo_projections_2022_2050.xlsx
+++ b/projections/aeo_projections_2022_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06746B86-2C59-436E-819C-CC796F99097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D1029E6-1124-4975-8B55-56B8056B700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2484" yWindow="3576" windowWidth="17280" windowHeight="9960" tabRatio="865" firstSheet="1" activeTab="3" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="865" xr2:uid="{66FF5A79-9233-45F1-AB00-1D0D09C51BCE}"/>
   </bookViews>
   <sheets>
     <sheet name="fuel_price_factors_2022_2050" sheetId="9" r:id="rId1"/>
@@ -1263,9 +1263,6 @@
     <t>data_source</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
     <t>national</t>
   </si>
   <si>
@@ -1303,6 +1300,9 @@
   </si>
   <si>
     <t>AEO2022 Reference Case</t>
+  </si>
+  <si>
+    <t>policy_scenario</t>
   </si>
 </sst>
 </file>
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F5499C-249D-4660-AC39-83320A5A905A}">
   <dimension ref="A1:AG247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2224,13 +2224,13 @@
   <sheetData>
     <row r="1" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>393</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="D1" s="14">
         <v>2022</v>
@@ -2322,13 +2322,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>401</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D2" s="5">
         <f>aeo_fuel_price_projections!$F2/aeo_fuel_price_projections!$F2</f>
@@ -2449,13 +2449,13 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>401</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D3" s="5">
         <f>aeo_fuel_price_projections!$F3/aeo_fuel_price_projections!$F3</f>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>401</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>401</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>401</v>
@@ -2957,7 +2957,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>401</v>
@@ -3084,13 +3084,13 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>402</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D8" s="5">
         <f>aeo_fuel_price_projections!$F8/aeo_fuel_price_projections!$F8</f>
@@ -3211,13 +3211,13 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>402</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D9" s="5">
         <f>aeo_fuel_price_projections!$F9/aeo_fuel_price_projections!$F9</f>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>402</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>402</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>402</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>402</v>
@@ -3846,13 +3846,13 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>403</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D14" s="5">
         <f>aeo_fuel_price_projections!$F14/aeo_fuel_price_projections!$F14</f>
@@ -3973,13 +3973,13 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>403</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D15" s="5">
         <f>aeo_fuel_price_projections!$F15/aeo_fuel_price_projections!$F15</f>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>403</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>403</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>403</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>403</v>
@@ -4608,13 +4608,13 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>404</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D20" s="5">
         <f>aeo_fuel_price_projections!$F20/aeo_fuel_price_projections!$F20</f>
@@ -4735,13 +4735,13 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>404</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D21" s="5">
         <f>aeo_fuel_price_projections!$F21/aeo_fuel_price_projections!$F21</f>
@@ -4862,7 +4862,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>404</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>404</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>404</v>
@@ -5243,7 +5243,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>404</v>
@@ -5376,7 +5376,7 @@
         <v>401</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D26" s="5">
         <f>aeo_fuel_price_projections!$F26/aeo_fuel_price_projections!$F26</f>
@@ -6011,7 +6011,7 @@
         <v>401</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D31" s="5">
         <f>aeo_fuel_price_projections!$F31/aeo_fuel_price_projections!$F31</f>
@@ -6139,7 +6139,7 @@
         <v>402</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D32" s="5">
         <f>aeo_fuel_price_projections!$F32/aeo_fuel_price_projections!$F32</f>
@@ -6779,7 +6779,7 @@
         <v>402</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D37" s="5">
         <f>aeo_fuel_price_projections!$F37/aeo_fuel_price_projections!$F37</f>
@@ -6907,7 +6907,7 @@
         <v>403</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D38" s="5">
         <f>aeo_fuel_price_projections!$F38/aeo_fuel_price_projections!$F38</f>
@@ -7547,7 +7547,7 @@
         <v>403</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D43" s="5">
         <f>aeo_fuel_price_projections!$F43/aeo_fuel_price_projections!$F43</f>
@@ -7675,7 +7675,7 @@
         <v>404</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D44" s="5">
         <f>aeo_fuel_price_projections!$F44/aeo_fuel_price_projections!$F44</f>
@@ -8315,7 +8315,7 @@
         <v>404</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D49" s="5">
         <f>aeo_fuel_price_projections!$F49/aeo_fuel_price_projections!$F49</f>
@@ -8443,7 +8443,7 @@
         <v>401</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D50" s="5">
         <f>aeo_fuel_price_projections!$F50/aeo_fuel_price_projections!$F50</f>
@@ -9081,7 +9081,7 @@
         <v>401</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D55" s="5">
         <f>aeo_fuel_price_projections!$F55/aeo_fuel_price_projections!$F55</f>
@@ -9208,7 +9208,7 @@
         <v>402</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D56" s="5">
         <f>aeo_fuel_price_projections!$F56/aeo_fuel_price_projections!$F56</f>
@@ -9843,7 +9843,7 @@
         <v>402</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D61" s="5">
         <f>aeo_fuel_price_projections!$F61/aeo_fuel_price_projections!$F61</f>
@@ -9970,7 +9970,7 @@
         <v>403</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D62" s="5">
         <f>aeo_fuel_price_projections!$F62/aeo_fuel_price_projections!$F62</f>
@@ -10605,7 +10605,7 @@
         <v>403</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D67" s="5">
         <f>aeo_fuel_price_projections!$F67/aeo_fuel_price_projections!$F67</f>
@@ -10732,7 +10732,7 @@
         <v>404</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D68" s="5">
         <f>aeo_fuel_price_projections!$F68/aeo_fuel_price_projections!$F68</f>
@@ -11367,7 +11367,7 @@
         <v>404</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D73" s="5">
         <f>aeo_fuel_price_projections!$F73/aeo_fuel_price_projections!$F73</f>
@@ -11494,7 +11494,7 @@
         <v>401</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D74" s="5">
         <f>aeo_fuel_price_projections!$F74/aeo_fuel_price_projections!$F74</f>
@@ -12129,7 +12129,7 @@
         <v>401</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D79" s="5">
         <f>aeo_fuel_price_projections!$F79/aeo_fuel_price_projections!$F79</f>
@@ -12256,7 +12256,7 @@
         <v>402</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D80" s="5">
         <f>aeo_fuel_price_projections!$F80/aeo_fuel_price_projections!$F80</f>
@@ -12891,7 +12891,7 @@
         <v>402</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D85" s="5">
         <f>aeo_fuel_price_projections!$F85/aeo_fuel_price_projections!$F85</f>
@@ -13018,7 +13018,7 @@
         <v>403</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D86" s="5">
         <f>aeo_fuel_price_projections!$F86/aeo_fuel_price_projections!$F86</f>
@@ -13653,7 +13653,7 @@
         <v>403</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D91" s="5">
         <f>aeo_fuel_price_projections!$F91/aeo_fuel_price_projections!$F91</f>
@@ -13780,7 +13780,7 @@
         <v>404</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D92" s="5">
         <f>aeo_fuel_price_projections!$F92/aeo_fuel_price_projections!$F92</f>
@@ -14415,7 +14415,7 @@
         <v>404</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D97" s="5">
         <f>aeo_fuel_price_projections!$F97/aeo_fuel_price_projections!$F97</f>
@@ -14542,7 +14542,7 @@
         <v>401</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D98" s="5">
         <f>aeo_fuel_price_projections!$F98/aeo_fuel_price_projections!$F98</f>
@@ -15177,7 +15177,7 @@
         <v>401</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D103" s="5">
         <f>aeo_fuel_price_projections!$F103/aeo_fuel_price_projections!$F103</f>
@@ -15304,7 +15304,7 @@
         <v>402</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D104" s="5">
         <f>aeo_fuel_price_projections!$F104/aeo_fuel_price_projections!$F104</f>
@@ -15939,7 +15939,7 @@
         <v>402</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D109" s="5">
         <f>aeo_fuel_price_projections!$F109/aeo_fuel_price_projections!$F109</f>
@@ -16066,7 +16066,7 @@
         <v>403</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D110" s="5">
         <f>aeo_fuel_price_projections!$F110/aeo_fuel_price_projections!$F110</f>
@@ -16701,7 +16701,7 @@
         <v>403</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D115" s="5">
         <f>aeo_fuel_price_projections!$F115/aeo_fuel_price_projections!$F115</f>
@@ -16828,7 +16828,7 @@
         <v>404</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D116" s="5">
         <f>aeo_fuel_price_projections!$F116/aeo_fuel_price_projections!$F116</f>
@@ -17463,7 +17463,7 @@
         <v>404</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D121" s="5">
         <f>aeo_fuel_price_projections!$F121/aeo_fuel_price_projections!$F121</f>
@@ -17590,7 +17590,7 @@
         <v>401</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D122" s="5">
         <f>aeo_fuel_price_projections!$F122/aeo_fuel_price_projections!$F122</f>
@@ -18225,7 +18225,7 @@
         <v>401</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D127" s="5">
         <f>aeo_fuel_price_projections!$F127/aeo_fuel_price_projections!$F127</f>
@@ -18352,7 +18352,7 @@
         <v>402</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D128" s="5">
         <f>aeo_fuel_price_projections!$F128/aeo_fuel_price_projections!$F128</f>
@@ -18987,7 +18987,7 @@
         <v>402</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D133" s="5">
         <f>aeo_fuel_price_projections!$F133/aeo_fuel_price_projections!$F133</f>
@@ -19114,7 +19114,7 @@
         <v>403</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D134" s="5">
         <f>aeo_fuel_price_projections!$F134/aeo_fuel_price_projections!$F134</f>
@@ -19749,7 +19749,7 @@
         <v>403</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D139" s="5">
         <f>aeo_fuel_price_projections!$F139/aeo_fuel_price_projections!$F139</f>
@@ -19876,7 +19876,7 @@
         <v>404</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D140" s="5">
         <f>aeo_fuel_price_projections!$F140/aeo_fuel_price_projections!$F140</f>
@@ -20511,7 +20511,7 @@
         <v>404</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D145" s="5">
         <f>aeo_fuel_price_projections!$F145/aeo_fuel_price_projections!$F145</f>
@@ -20638,7 +20638,7 @@
         <v>401</v>
       </c>
       <c r="C146" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D146" s="5">
         <f>aeo_fuel_price_projections!$F146/aeo_fuel_price_projections!$F146</f>
@@ -21273,7 +21273,7 @@
         <v>401</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D151" s="5">
         <f>aeo_fuel_price_projections!$F151/aeo_fuel_price_projections!$F151</f>
@@ -21400,7 +21400,7 @@
         <v>402</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D152" s="5">
         <f>aeo_fuel_price_projections!$F152/aeo_fuel_price_projections!$F152</f>
@@ -22035,7 +22035,7 @@
         <v>402</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D157" s="5">
         <f>aeo_fuel_price_projections!$F157/aeo_fuel_price_projections!$F157</f>
@@ -22162,7 +22162,7 @@
         <v>403</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D158" s="5">
         <f>aeo_fuel_price_projections!$F158/aeo_fuel_price_projections!$F158</f>
@@ -22797,7 +22797,7 @@
         <v>403</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D163" s="5">
         <f>aeo_fuel_price_projections!$F163/aeo_fuel_price_projections!$F163</f>
@@ -22924,7 +22924,7 @@
         <v>404</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D164" s="5">
         <f>aeo_fuel_price_projections!$F164/aeo_fuel_price_projections!$F164</f>
@@ -23559,7 +23559,7 @@
         <v>404</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D169" s="5">
         <f>aeo_fuel_price_projections!$F169/aeo_fuel_price_projections!$F169</f>
@@ -23686,7 +23686,7 @@
         <v>401</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D170" s="5">
         <f>aeo_fuel_price_projections!$F170/aeo_fuel_price_projections!$F170</f>
@@ -24321,7 +24321,7 @@
         <v>401</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D175" s="5">
         <f>aeo_fuel_price_projections!$F175/aeo_fuel_price_projections!$F175</f>
@@ -24448,7 +24448,7 @@
         <v>402</v>
       </c>
       <c r="C176" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D176" s="5">
         <f>aeo_fuel_price_projections!$F176/aeo_fuel_price_projections!$F176</f>
@@ -25083,7 +25083,7 @@
         <v>402</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D181" s="5">
         <f>aeo_fuel_price_projections!$F181/aeo_fuel_price_projections!$F181</f>
@@ -25210,7 +25210,7 @@
         <v>403</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D182" s="5">
         <f>aeo_fuel_price_projections!$F182/aeo_fuel_price_projections!$F182</f>
@@ -25845,7 +25845,7 @@
         <v>403</v>
       </c>
       <c r="C187" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D187" s="5">
         <f>aeo_fuel_price_projections!$F187/aeo_fuel_price_projections!$F187</f>
@@ -25972,7 +25972,7 @@
         <v>404</v>
       </c>
       <c r="C188" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D188" s="5">
         <f>aeo_fuel_price_projections!$F188/aeo_fuel_price_projections!$F188</f>
@@ -26607,7 +26607,7 @@
         <v>404</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D193" s="5">
         <f>aeo_fuel_price_projections!$F193/aeo_fuel_price_projections!$F193</f>
@@ -26734,7 +26734,7 @@
         <v>401</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D194" s="5">
         <f>aeo_fuel_price_projections!$F194/aeo_fuel_price_projections!$F194</f>
@@ -27369,7 +27369,7 @@
         <v>401</v>
       </c>
       <c r="C199" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D199" s="5">
         <f>aeo_fuel_price_projections!$F199/aeo_fuel_price_projections!$F199</f>
@@ -27496,7 +27496,7 @@
         <v>402</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D200" s="5">
         <f>aeo_fuel_price_projections!$F200/aeo_fuel_price_projections!$F200</f>
@@ -28131,7 +28131,7 @@
         <v>402</v>
       </c>
       <c r="C205" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D205" s="5">
         <f>aeo_fuel_price_projections!$F205/aeo_fuel_price_projections!$F205</f>
@@ -28258,7 +28258,7 @@
         <v>403</v>
       </c>
       <c r="C206" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D206" s="5">
         <f>aeo_fuel_price_projections!$F206/aeo_fuel_price_projections!$F206</f>
@@ -28893,7 +28893,7 @@
         <v>403</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D211" s="5">
         <f>aeo_fuel_price_projections!$F211/aeo_fuel_price_projections!$F211</f>
@@ -29020,7 +29020,7 @@
         <v>404</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D212" s="5">
         <f>aeo_fuel_price_projections!$F212/aeo_fuel_price_projections!$F212</f>
@@ -29655,7 +29655,7 @@
         <v>404</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D217" s="5">
         <f>aeo_fuel_price_projections!$F217/aeo_fuel_price_projections!$F217</f>
@@ -29782,7 +29782,7 @@
         <v>401</v>
       </c>
       <c r="C218" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D218" s="5">
         <f>aeo_fuel_price_projections!$F218/aeo_fuel_price_projections!$F218</f>
@@ -30417,7 +30417,7 @@
         <v>401</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D223" s="5">
         <f>aeo_fuel_price_projections!$F223/aeo_fuel_price_projections!$F223</f>
@@ -30544,7 +30544,7 @@
         <v>402</v>
       </c>
       <c r="C224" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D224" s="5">
         <f>aeo_fuel_price_projections!$F224/aeo_fuel_price_projections!$F224</f>
@@ -31179,7 +31179,7 @@
         <v>402</v>
       </c>
       <c r="C229" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D229" s="5">
         <f>aeo_fuel_price_projections!$F229/aeo_fuel_price_projections!$F229</f>
@@ -31306,7 +31306,7 @@
         <v>403</v>
       </c>
       <c r="C230" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D230" s="5">
         <f>aeo_fuel_price_projections!$F230/aeo_fuel_price_projections!$F230</f>
@@ -31941,7 +31941,7 @@
         <v>403</v>
       </c>
       <c r="C235" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D235" s="5">
         <f>aeo_fuel_price_projections!$F235/aeo_fuel_price_projections!$F235</f>
@@ -32068,7 +32068,7 @@
         <v>404</v>
       </c>
       <c r="C236" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D236" s="5">
         <f>aeo_fuel_price_projections!$F236/aeo_fuel_price_projections!$F236</f>
@@ -32703,7 +32703,7 @@
         <v>404</v>
       </c>
       <c r="C241" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D241" s="5">
         <f>aeo_fuel_price_projections!$F241/aeo_fuel_price_projections!$F241</f>
@@ -33012,7 +33012,7 @@
   <dimension ref="A1:AI241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33025,7 +33025,7 @@
   <sheetData>
     <row r="1" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>393</v>
@@ -33034,7 +33034,7 @@
         <v>406</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>6</v>
@@ -33129,7 +33129,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>401</v>
@@ -33233,7 +33233,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>401</v>
@@ -33337,7 +33337,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>401</v>
@@ -33441,7 +33441,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>401</v>
@@ -33545,7 +33545,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>401</v>
@@ -33649,7 +33649,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>401</v>
@@ -33753,7 +33753,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>402</v>
@@ -33857,7 +33857,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>402</v>
@@ -33961,7 +33961,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>402</v>
@@ -34065,7 +34065,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>402</v>
@@ -34169,7 +34169,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>402</v>
@@ -34273,7 +34273,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>402</v>
@@ -34377,7 +34377,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>403</v>
@@ -34481,7 +34481,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>403</v>
@@ -34585,7 +34585,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>403</v>
@@ -34689,7 +34689,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>403</v>
@@ -34793,7 +34793,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>403</v>
@@ -34897,7 +34897,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>403</v>
@@ -35001,7 +35001,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>404</v>
@@ -35105,7 +35105,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>404</v>
@@ -35209,7 +35209,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>404</v>
@@ -35313,7 +35313,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>404</v>
@@ -35417,7 +35417,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>404</v>
@@ -35521,7 +35521,7 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>404</v>
@@ -58133,7 +58133,7 @@
   <sheetData>
     <row r="1" spans="1:34" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B1" s="14">
         <v>2018</v>
@@ -58237,7 +58237,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B2" s="13">
         <f>aeo_hdd_projections!$F2/aeo_hdd_projections!$F2</f>
@@ -59645,8 +59645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B2126A-7C3E-492E-A994-6660270B8389}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59656,7 +59656,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B1" s="14">
         <v>2022</v>
@@ -59748,7 +59748,7 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B2" s="13">
         <f>aeo_hdd_projections!$J2/aeo_hdd_projections!$J2</f>
@@ -61008,19 +61008,19 @@
   <sheetData>
     <row r="1" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>417</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F1" s="14">
         <v>2018</v>
@@ -61124,19 +61124,19 @@
     </row>
     <row r="2" spans="1:38" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E2" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F2" s="12">
         <v>4291</v>
@@ -61243,16 +61243,16 @@
         <v>233</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F3" s="12">
         <v>6434</v>
@@ -61359,16 +61359,16 @@
         <v>242</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F4" s="12">
         <v>3479</v>
@@ -61475,16 +61475,16 @@
         <v>230</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F5" s="12">
         <v>5769</v>
@@ -61591,16 +61591,16 @@
         <v>248</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F6" s="12">
         <v>4808</v>
@@ -61707,16 +61707,16 @@
         <v>226</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F7" s="12">
         <v>6323</v>
@@ -61823,16 +61823,16 @@
         <v>251</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F8" s="12">
         <v>3172</v>
@@ -61939,16 +61939,16 @@
         <v>239</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F9" s="12">
         <v>2638</v>
@@ -62055,16 +62055,16 @@
         <v>236</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F10" s="12">
         <v>6974</v>
@@ -62171,16 +62171,16 @@
         <v>245</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>411</v>
-      </c>
       <c r="E11" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F11" s="12">
         <v>2252</v>

</xml_diff>